<commit_message>
Criação de tópicos contendo artigos relevantes para cada tópico - Continuidade de leitura
</commit_message>
<xml_diff>
--- a/FICHAMENTO.xlsx
+++ b/FICHAMENTO.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m23884\Documents\GitHub\weak_signals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigosantos/Documents/GitHub/weak_signals/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323F3ADE-D858-4D4B-9986-F18F09F69E27}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4155" yWindow="-21135" windowWidth="36675" windowHeight="21135"/>
+    <workbookView xWindow="-4160" yWindow="-21140" windowWidth="36680" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -19,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="110">
   <si>
     <t>Título</t>
   </si>
@@ -434,7 +429,16 @@
 PERSPECTIVE OF INTELLIGENCE</t>
   </si>
   <si>
-    <t>@inproceedings{inproceedings,
+    <t>3</t>
+  </si>
+  <si>
+    <t>Mas o empreender, no contexto de competitividade empresarial, tem se aproximado intensamente da capacidade da orgnanização em monitorar o ambiente de negócios, definindo claramente a gestão da informação capaz de lhe assegurar um posicionamento superior no mercado.</t>
+  </si>
+  <si>
+    <t>Sinais fracos</t>
+  </si>
+  <si>
+    <t>@inproceedings{2014MunizMery,
 author = {Muniz, Raquel and Blanck, Mery},
 year = {2014},
 month = {05},
@@ -445,19 +449,22 @@
 }</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Mas o empreender, no contexto de competitividade empresarial, tem se aproximado intensamente da capacidade da orgnanização em monitorar o ambiente de negócios, definindo claramente a gestão da informação capaz de lhe assegurar um posicionamento superior no mercado.</t>
-  </si>
-  <si>
-    <t>Sinais fracos</t>
+    <t>Weak Signals Management</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Sobretudo, os aspectos relativos à informação são importantes na medida em que se constata que é exatamente a partir dos dados, do significado da informação que resulta destes e do conhecimento advindo a partir da compreensão, entendimento e aprendizado proporcionados pelo conhecimento que a Inteligência pode se estabelecer.</t>
+  </si>
+  <si>
+    <t>Sobre informações e conhecimento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -837,29 +844,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="107" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="86.625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="31.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="86.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="6.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="5.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="27.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="233.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.875" style="5"/>
+    <col min="4" max="4" width="47.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="27.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="233.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -891,7 +898,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="42" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -913,7 +920,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="70" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
@@ -931,7 +938,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="42" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
@@ -952,7 +959,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="42" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
@@ -973,7 +980,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="70" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
@@ -991,7 +998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="98" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
@@ -1006,7 +1013,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="42" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
@@ -1024,7 +1031,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="56" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1042,7 +1049,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="140" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>29</v>
       </c>
@@ -1060,7 +1067,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="140" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
@@ -1078,7 +1085,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="102" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="126" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -1102,7 +1109,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="28" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
@@ -1113,12 +1120,14 @@
         <v>86</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="G13" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H13" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="70" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
@@ -1129,23 +1138,28 @@
         <v>87</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="G14" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H14" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="28" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="6">
         <v>3</v>
       </c>
+      <c r="G15" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H15" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="56" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
@@ -1155,11 +1169,14 @@
       <c r="D16" s="2" t="s">
         <v>88</v>
       </c>
+      <c r="G16" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H16" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="56" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
@@ -1169,11 +1186,14 @@
       <c r="D17" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="G17" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H17" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="112" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
@@ -1183,11 +1203,14 @@
       <c r="D18" s="2" t="s">
         <v>90</v>
       </c>
+      <c r="G18" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H18" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="42" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -1197,11 +1220,14 @@
       <c r="D19" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="G19" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H19" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="112" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>47</v>
       </c>
@@ -1211,11 +1237,14 @@
       <c r="D20" s="2" t="s">
         <v>92</v>
       </c>
+      <c r="G20" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H20" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="56" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>46</v>
       </c>
@@ -1225,55 +1254,70 @@
       <c r="D21" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="G21" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H21" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>52</v>
       </c>
+      <c r="G22" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H22" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="84" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="G23" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H23" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="112" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>61</v>
       </c>
+      <c r="G24" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H24" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="102" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="112" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="G25" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H25" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="42" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>66</v>
       </c>
@@ -1283,11 +1327,14 @@
       <c r="D26" s="2" t="s">
         <v>94</v>
       </c>
+      <c r="G26" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H26" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" ht="98" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>68</v>
       </c>
@@ -1297,11 +1344,14 @@
       <c r="D27" s="2" t="s">
         <v>95</v>
       </c>
+      <c r="G27" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H27" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="84" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>70</v>
       </c>
@@ -1311,11 +1361,14 @@
       <c r="D28" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="G28" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H28" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" ht="98" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>73</v>
       </c>
@@ -1325,11 +1378,14 @@
       <c r="D29" s="2" t="s">
         <v>97</v>
       </c>
+      <c r="G29" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H29" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" ht="70" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>77</v>
       </c>
@@ -1339,11 +1395,14 @@
       <c r="D30" s="2" t="s">
         <v>98</v>
       </c>
+      <c r="G30" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H30" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" ht="84" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>78</v>
       </c>
@@ -1353,16 +1412,22 @@
       <c r="D31" s="2" t="s">
         <v>99</v>
       </c>
+      <c r="G31" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H31" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="204" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" ht="238" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+      <c r="G32" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>84</v>
       </c>
@@ -1372,25 +1437,45 @@
       <c r="D33" s="2" t="s">
         <v>100</v>
       </c>
+      <c r="G33" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="H33" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="84" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>101</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="G34" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H34" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="I34" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="I34" s="4" t="s">
-        <v>102</v>
+    </row>
+    <row r="35" spans="1:9" ht="84" x14ac:dyDescent="0.2">
+      <c r="C35" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Leituras e mais leituras
</commit_message>
<xml_diff>
--- a/FICHAMENTO.xlsx
+++ b/FICHAMENTO.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigosantos/Documents/GitHub/weak_signals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4085414E-A588-E24C-A7FF-D79C3CA12135}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C4BBF6-8AE4-E046-9ED8-379E8E4F1598}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4160" yWindow="-21140" windowWidth="36680" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4060" yWindow="-21000" windowWidth="36680" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="159">
   <si>
     <t>Título</t>
   </si>
@@ -469,6 +468,161 @@
   </si>
   <si>
     <t>Apud - Cooper, D. R., &amp; Schindler, P. S. (2004). Métodos de pesquisa em administração (7a ed.). Porto Alegre, RS: Artmed.</t>
+  </si>
+  <si>
+    <t>Cenários prospectivos: Como construir um futuro melhor</t>
+  </si>
+  <si>
+    <t>A ciência, em particular, mais do que fonte de verdades universais soibre o mundo natural, deve ser também dinâmica e engajada nos mecanismos de criação da ordem epistemológica das sociedades modernas.</t>
+  </si>
+  <si>
+    <t>O futuro funda-se no que fazemos no presente.</t>
+  </si>
+  <si>
+    <t>Devemos considerar a prospecção um processo continuado de pensar o futuro e de identificar elementos para a melhor tomada de decisão, levando em consideração aspectos econômicos, sociais, ambientais, cinetíficos e tecnológicos. Não se trata, pois, de explorar faculdades divinatórias. Cenários não são predições sobre o que irá acontecer, mas descrições, com base em hipóteses plausíveis, o que poderá acontecer. A premissa é de que o futuro não está, em larga margem, pre-determinado e, portanto, pode ser moldado pela ação dos atores sociais.</t>
+  </si>
+  <si>
+    <t>Como nunca no passado, é indispensável que o Brasil pense  e planeje o seu futuro, buscando as condições que o levem ao progresso de maneira favorável. O passado, aliás, deve também nos servir como orientador desses exercícios, porque se reflete na própria atualidade brasileira, na qual convivem o arcaico e o inovador, o saudosismo e o eterno devir.</t>
+  </si>
+  <si>
+    <t>Esse ambiente turbulento e repleto de rupeturas de tendÊncia, que impedem a utilização dos modelos clássicos de previsão e projeções, está se revelando um campo propício para diversas críticas que desqualificam os estudos ligados ao futuro.</t>
+  </si>
+  <si>
+    <t>Prefácio</t>
+  </si>
+  <si>
+    <t>Introdução</t>
+  </si>
+  <si>
+    <t>Será que previsões falharam, ou foi a mão do homem, que, tendo conhecimento delas com antecedência e sabendo de suas consequências, mudou o curso da história, tomando providÊncias para que não ocorressem?</t>
+  </si>
+  <si>
+    <t>Os estudos prospectivos não têm como objetivo prever o futuro e, sim, estudar as diversas possibilidades de futuros plausíveis existentes e preparar as organizações para enfrentar qualquer uma delas, ou até mesmo criar condições para que modifiquem suas probabilidades de ocorrÊncia, ou minimizar seus efeitos. Apesar de serem muitas vezes confundidos com previsões ou projeções, trat-se de estudos do futuro com abordagem completamente diferente.</t>
+  </si>
+  <si>
+    <t>Prospecção</t>
+  </si>
+  <si>
+    <t>No contexto da inteligência competitiva, os cenários prospectivos são considerados uma das ferramentas de análise mais importantes para a definição de estratégias em ambientes cada vez mais turbulentos e incertos.</t>
+  </si>
+  <si>
+    <t>Verifica-se também que a definição de estratégias não é a única contribuição que os estudos de cenários podem prestar às organizações. Outros tipos de contribuiçção são a unificação da linguagem da organização, o auxílio no desenvolvimento de sua criatividade, a criação de redes de informação, o aprendizado organizacional, um melhor entendimento do ambiente que cerca a organização e de sua atuação em ambientes de grande incerteza.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cenários </t>
+  </si>
+  <si>
+    <t>Segunto Rattner (1979), a especulação é um discurso sobre o futuro, no qual seu aturor admite incerteza e/ou falta de poio lógico-racional, substituído por opiniões vagas e imaginação fértil.</t>
+  </si>
+  <si>
+    <t>Em nossa vida cotidiana, os fatos já conhecidos são a principal "matéria-prima" para o estabelecimento de nosso planejamento diário.</t>
+  </si>
+  <si>
+    <t>O medo foi, portanto, o principal agente que obrigou a humanidade a mudar de atitude em relação ao futuro, ao fazer com que ela deixasse de ser uma mea espectadora da história e passasse a ter particiapção ativa na construção de seu futuro na Terra.</t>
+  </si>
+  <si>
+    <t>Prospecção - Motivações</t>
+  </si>
+  <si>
+    <t>Apesar das preocupações em evitar uma catástrofe mundial, foram dois fatores conjunturais os princpais motivadores do surgimento de novas metodologias que viabilizassem um melhor planejamento estratégico: a gerra gria e a resonstrução da França.</t>
+  </si>
+  <si>
+    <t>Prospeção - Futuro</t>
+  </si>
+  <si>
+    <t>A finalidade dos cenários exploratórios era "ampliar a compreensão do sistema, identificar os elemntos predeterminados e descobrir as conexões entre as várias forças e eventos que conduziam esse sistema", o que levaria, consequentemente, a uma melhor tomada de decisão.</t>
+  </si>
+  <si>
+    <t>Cenários - Finalidade</t>
+  </si>
+  <si>
+    <t>Cenários - Contribuição</t>
+  </si>
+  <si>
+    <t>Também argumenta que, apesar de existirem questões ligadas ao futuro que não podem ser evitadas, isso não significa que se deva ficar parado, esperando que elas aconteçam.</t>
+  </si>
+  <si>
+    <t>Os estudos de cenários prospectivos são uma das ferramentas mais adequadas para a definição de estratégias em ambientes turbulentos e incertos. Embora a prospectiva não se proponha eliminar essas incertezas, aponta meios de reduzi-las, possibilitando tomadas de decisão fundamentas em futuros hipotéticos.</t>
+  </si>
+  <si>
+    <t>Porter (1992) e Schwartz (1996) sugerem que, como uma empresa não sabe de antemão que cenários deve ocorrer em função das incertezas do ambiente, deve optar pela definição de estratégias robustas que sejam satisfatórias em qualquer cenário real. Porde-se citar como exemplo extremo o caso da SCE (1992), que elaborou 12 cenários para desenvolver uma estratégia o mais robusta possível. Segundo Schwartz, é importante que os administradores vivenciem cada cenários e definam que estratégias ou ações devem ser adotadas em cada um deles para que a empresa tenha sucesso, independetemente do cenário.</t>
+  </si>
+  <si>
+    <t>Cenários - Como usar</t>
+  </si>
+  <si>
+    <t>Marcial sugere três posturas para as organizações em relação ao futuro, que é múltiplo e incerto, onde os atores - agentes de mudança - podem vir a modificá-lo: 
+- Construtora do futuro: a organização é líder de mercado no assunto em pauta, tem velocidade e recursos para "contra-atacar" e vale a pena tal investimento. Sendo assim, ações deverão ser realizadas no sentido de a empresa construir o futuro a seu favor, minimnizando ou eliminando o risco do movimento identificado, ou aproveitando ao máximo as oportnidades vislumbradas;
+- Influenciadora da construção do futuro: a organização não tem condições de construir o futuro, mas pode influenciar sua construção, em função de suas ligações com atores que possuem essa força. Além disso, está evidenciado que é importante para a empresa influenciar o curso dos acontecimentos. Sendo assim, ações devem ser desenvolvidas para que este seja alterado a seu favor, por intermédio do convencimento dos atores que tÊm o poder de construir o futuro. A atuação da empresa para reforçar a ação de seus parceiros também se constitui em movimento importante nessa situação;
+- gerenciadora do risco: a organização não tem condições de construir o futuro, ou considera que não vale a pena um movimento nesse sentido, em funçao dos custos envolvidos. Também não tem como influenciar essa construção. Então, ações deverão ser realizadas, no sentido de reduzir o risco em relação ao futuro, prevenindo-se quanto às ameaças.</t>
+  </si>
+  <si>
+    <t>Prospecção - Posturas</t>
+  </si>
+  <si>
+    <t>Mais importante do que buscar acertar o que vai acontecer é construir cenários que forneçam informações importantes a respeito das possibiliades de futuro e, assim, auxiliem na construção do futuro desejado.</t>
+  </si>
+  <si>
+    <t>Modelos menatis são imagens internas profundamente arraigadas sobre o funcionamento do mundo, imagens que nos limitam a formas bem conhecidas de pensar e agir. São os modelos mentais que nos levam a reagir de maneiras diferentes ao mesmo acontecimento ou a descrever de forma diferente o mesmo evento observado, São os modelos mentais que levam as pessoas a observar o mundo de modo diferente e a reagir de forma diferente ao mesmo acontecimento, Observamos sempre o mundo à nossa volta segundo nossos modelos mentais, e são eles que determinam não só como entendemos o mundo, mas também como agimos e reagimos aos acontecimentos.</t>
+  </si>
+  <si>
+    <t>Sinais Fracos - Mindset</t>
+  </si>
+  <si>
+    <t>A definiçãpo mais abrangente e acadêmica encontrada na literatura é a de Michel Godet (1987), para quem cenário é "o conjunto formado pela descrição coerente de uma situação futura e pelo encaminhamento dos acontecimentos que permitem passar da situação de origem à situação futura"</t>
+  </si>
+  <si>
+    <t>Cenários - Conceito</t>
+  </si>
+  <si>
+    <t>Godet complementa a sua definição afirmando que um cenários não é a realidade futura, mas um meio de representá-la, com o objetivo de nortear a ação presente, à luz dos futuros possíveis e desejáveis.</t>
+  </si>
+  <si>
+    <t>No que diz respeito ao conteúdo de um cenário, primeiramente deve-se considerar o sistema em que a organização atua. Esse sistema é composto pelo objetivo de cearização, seu horizonte temporal e lugar (figura 3). O sistemna é visto como uma totalidade organizada em elementos e fenômenos interligados e interdependentes, que podem formar sistemas menores ou subsistemas daquele que está sendo considerado.</t>
+  </si>
+  <si>
+    <t>O horizonte de tempo do cenário é o período coberto pelo estudo de cenarização. Pode variar em função da dinâmica e da evolução do sistema estudado, mas, em média, deve ser de 10 anos,. É recomendável que os cenários não tenham um horizonte temporal inferior a cinco anos. Essa limitação está relacionada com o objetivo principal dos cenários - auxiliar na definiçãodas estratégias da empresa -, o que exige uma abordagem de longo prazo.</t>
+  </si>
+  <si>
+    <t>Um cenário completo em geral contém seis componentes principais: um título, uma filosofia, variáveis, atores, cenas e trajetória.</t>
+  </si>
+  <si>
+    <t>Em qualquer cenários, o título, segudno Schwartz (1996), "é possuidor de uma carga tremenda, pois age como sua referência",. Ele serve como lembrança ou referência de um cenário específico.
+A filosofia sintetiza o movimento ou a direção fundamental do sistema considerado., Ela constitui a ideia - força do cenário.
+As variáveis representam aspectos ou elementos relevantes do sistema ou do contexto considerado, tendo em vista o objetivo do cenário.
+Os atores são indivíduos, grupos, decisores, organizações ou associações de classe que influenciam ou rece bem influência significativa do sistema e/ou contexto considerado no cenário.
+A cena é uma visão da situação considerada em um determinado instante do tempo, a qual descreve como estão organizados ou vinculados entre si os atores e as variáveis naquele instante.
+Trajetória é o percurso ou caminho seguido pelo sistemq no horizonte de tempo considerado.</t>
+  </si>
+  <si>
+    <t>Um cenário possui diversas características. A mai simportante é a visão plural do futuro (como este não está escrito, parte-se do pressuposto de que existem vários futuros)</t>
+  </si>
+  <si>
+    <t>Outra característica interessante dos cenários é o fato de não poderem ser "encomendados" externamente. Para serem efetivos, os cenários devem ser desenvolvidos dentro da organização.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cenáros </t>
+  </si>
+  <si>
+    <t>Quanto a tipologia, os cenários são qualificados por sua natureza ou probabilidade e podem ser classificados como normativos ou exploratórios. 
+Cenários normativos são aqueles que configuram futuros desejados, exprimindo sempre o compromisso de um ou mais atores com a consecução de determinados objetivos e projetos ou com a superação de desafios empresariais ou tecnológicos. A lógica de construção desses cenários consiste em estabelecer primeiro, o futuro desejado para, depois, traçar as trajetórias para alcança-lo.
+Os cenários exploratórios caracterizam-se por futuros possíveis ou prováveis do sistema considerado e/ou de seu contexto, mediante a simulação e o desenvolvimento de certas condições iniciais</t>
+  </si>
+  <si>
+    <t>Verifica-se que o número de cenários deve ser escolhido de acordo com o perfil da empresa e os objetivos a serem alcaçados. O objetivo deve ser a exploração dos futuros possíveis e a análise de seus impactos na empresa, O número mais indicado é aquele que facilita a definição das estratégias da empresa e não complica o processo.</t>
+  </si>
+  <si>
+    <t>Um dos desafios enfrentados pelos profissionais que estudam o futuro é a identificação das "sementes de futuro" (Marcial, 2004). Segundo Marcial, o futuro deixa, no passado e no presente, sementes que podem vir a germinar ou não. Que podem se transformar em belas árvores frutíferas, plantas que nunca darão frutos ou mesmo plantas daninhas.</t>
+  </si>
+  <si>
+    <t>Marcial considera sementes de futuro os seguintes elementos: invariantes, tendÊncias de peso, elemntos predeterminados, fatos portadores de futuro, incertezas críticas, surpresas inevitáveis, wild cards - coringas e atores.
+Atores - são os atores que podem mudar o curso dos acontecimentos, mesmo em eventos em que não podem impedir sua ocorrência.
+Tendências de peso - eventos cuja perspectiva de direção é suficientemente consolidada e visível para se admitir sua permanência no período considerado. São movimentos muito prováveis de uma tor ou variável dentro do horizonte do cenário.
+Fatos ou elementos predeterminados - eventos já conhecidos e certos, cuja solução ou controle pelo sistema ainda não se efetivou.
+Fatos portadores de futuro - constituem-se em sinais ínfimos, por sua dimnensão presente,m existentes no abiente, mas imnensos por suas consequeêçncias e potencialidades. São esses fatos, existentes no ambiente, que podem sinalizar a existência de incertezas críticas, de surpresas inevitáveis ou de coringas (wild cards). Cabe chamar a atenção quanto à importância de identificar e analisar os fatos portadores de futuro, visto que são eles que possibilitam, muitas vezes, às organiações, moldarem o futuro de acordo com suas estratégias. Ao contrário das tendências de peso, esses fatos ainda não sinalizaram seu comportamento futuro; sendo assim a organização tem mais condições de moldá-lo a seu favor. Os fatos portadores de futuro são sementes importantes a serem identificadas durante os estudos de futuro, principalmente nos processos de construção de cenários, pois determinam sua lógica, e sinalizam a existência de outras sementes.
+Incertezas críticas - constituem-se nmaquelas variáveis incertas que são de grande importância para a questão principal. Pode-se dizer que se constituem naqueles fatos portadores de futuro considerados mais importantes e com grau de incerteza maior para a questão principal, ou seja, aqueles que determinam a construção dos cenários.
+Surpresas inevitáveis - forças previsíveis, pois têm suas raízes em forças que já estão em opração neste momento, mas não se sabe quando irão se configurar nem podemos conhecer previamente suas consequências e como nos afetarão. Geralmente são classificadas erroneamente como tendências.
+Coringas ou wild cards - referem-se às grandes surpresas, difíceis de serem antecipadas ou entendidas. possuem pequena probabilidade de ocorrência, são de grande impacto, e "geralmente surpreendem a todos, em parte porque se materializam muito rapidamente, tão rapidamente que sistemas sociais não podem efetivamente respondê-los". Por suas características intrínsecas, para a maioria dos coringas as únicas ações que podemos desenvolver hoje em dia são os planos de contingência.</t>
   </si>
 </sst>
 </file>
@@ -501,12 +655,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -521,7 +681,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -539,6 +699,18 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -855,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="107" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="107" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1412,7 +1584,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="84" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" ht="98" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>78</v>
       </c>
@@ -1437,7 +1609,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>84</v>
       </c>
@@ -1454,7 +1626,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="84" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="84" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>101</v>
       </c>
@@ -1474,7 +1646,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="98" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="98" x14ac:dyDescent="0.2">
       <c r="C35" s="4" t="s">
         <v>107</v>
       </c>
@@ -1488,7 +1660,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="56" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="56" x14ac:dyDescent="0.2">
       <c r="D36" s="2" t="s">
         <v>110</v>
       </c>
@@ -1500,6 +1672,376 @@
       </c>
       <c r="I36" s="4" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" s="9" customFormat="1" ht="56" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+    </row>
+    <row r="38" spans="1:10" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+    </row>
+    <row r="39" spans="1:10" s="9" customFormat="1" ht="154" x14ac:dyDescent="0.2">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+    </row>
+    <row r="40" spans="1:10" s="9" customFormat="1" ht="98" x14ac:dyDescent="0.2">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+    </row>
+    <row r="41" spans="1:10" ht="70" x14ac:dyDescent="0.2">
+      <c r="D41" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="56" x14ac:dyDescent="0.2">
+      <c r="D42" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="126" x14ac:dyDescent="0.2">
+      <c r="D43" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="56" x14ac:dyDescent="0.2">
+      <c r="D44" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="126" x14ac:dyDescent="0.2">
+      <c r="D45" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="56" x14ac:dyDescent="0.2">
+      <c r="D46" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="42" x14ac:dyDescent="0.2">
+      <c r="D47" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="70" x14ac:dyDescent="0.2">
+      <c r="D48" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="4:8" ht="70" x14ac:dyDescent="0.2">
+      <c r="D49" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="4:8" ht="84" x14ac:dyDescent="0.2">
+      <c r="D50" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="4:8" ht="56" x14ac:dyDescent="0.2">
+      <c r="D51" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="52" spans="4:8" ht="84" x14ac:dyDescent="0.2">
+      <c r="D52" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="4:8" ht="168" x14ac:dyDescent="0.2">
+      <c r="D53" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="4:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="D54" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="4:8" ht="56" x14ac:dyDescent="0.2">
+      <c r="D55" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="4:8" ht="182" x14ac:dyDescent="0.2">
+      <c r="D56" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="4:8" ht="84" x14ac:dyDescent="0.2">
+      <c r="D57" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="58" spans="4:8" ht="56" x14ac:dyDescent="0.2">
+      <c r="D58" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="59" spans="4:8" ht="112" x14ac:dyDescent="0.2">
+      <c r="D59" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="60" spans="4:8" ht="126" x14ac:dyDescent="0.2">
+      <c r="D60" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="4:8" ht="42" x14ac:dyDescent="0.2">
+      <c r="D61" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="62" spans="4:8" ht="345" x14ac:dyDescent="0.2">
+      <c r="D62" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="63" spans="4:8" ht="56" x14ac:dyDescent="0.2">
+      <c r="D63" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="64" spans="4:8" ht="56" x14ac:dyDescent="0.2">
+      <c r="D64" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="65" spans="4:8" ht="224" x14ac:dyDescent="0.2">
+      <c r="D65" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="66" spans="4:8" ht="84" x14ac:dyDescent="0.2">
+      <c r="D66" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="67" spans="4:8" ht="98" x14ac:dyDescent="0.2">
+      <c r="D67" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="68" spans="4:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="D68" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalização de leitura e atualização do fichamento
</commit_message>
<xml_diff>
--- a/FICHAMENTO.xlsx
+++ b/FICHAMENTO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\weak_signals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D570E8-70E0-40B9-A923-7AD458535FE0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C2B56D-191C-452A-8F98-B41FC6040435}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12825" yWindow="450" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6375" yWindow="2310" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="210">
   <si>
     <t>Título</t>
   </si>
@@ -707,6 +707,90 @@
   </si>
   <si>
     <t>No que diz respeito à elaboração de cenários prospectivos, vários autores, como Schwartz, Stffels e Wack, atribuem grande peso às fontes informais, pois estas possuem uma ligação maior com o futuro. Schwartz afirma que nessas fontes é que encontramos os sinais fracos que portam o futuro. O autor sugere que se mantenha contato com "notáveis", pensadores não convencionais, escritores e artistas em geral, porque essas pessoas extrapolam os especialistas e possuem uma visão mais holística e menos quantitativa do mundo.</t>
+  </si>
+  <si>
+    <t>@article{FonsecaEtAl2012,
+author = {Fonseca, Fernando and Mello Barreto, Luis Fernando},
+year = {2012},
+month = {01},
+pages = {34-58},
+title = {PROCESSO DECISÓRIO E O TRATAMENTO DE SINAIS FRACOS DOI:10.7444/fsrj.v3i2.80},
+volume = {3},
+journal = {Future Studies Research Journal: Trends and Strategies},
+doi = {10.24023/FutureJournal/2175-5825/2011.v3i2.80}
+}</t>
+  </si>
+  <si>
+    <t>Processo decisório e o tratamento de sinais fracos</t>
+  </si>
+  <si>
+    <t>Sinais Fracos</t>
+  </si>
+  <si>
+    <t>Sinais Fracos - Motivações</t>
+  </si>
+  <si>
+    <t>Um dos motivos da pouca difusão de práticas de monitoramento do ambiente para identificação e tratamento dos sinais fracos consiste no fato de que a natureza desta atividade se distancia das atividades foco do dia a dia dos gestores.</t>
+  </si>
+  <si>
+    <t>A informação coletada no ambiente, entendida como sinais fracos, é antecipatória, qualitativa, ambígua, fragmentada, pode vir em vários formatos e de várias fontes distrintas (...). Por esse motivo, a conceituação de sinais fracos prescinde de uma estrutura formal, ou de um processo estrabelecido, onde não basta somente a captação dos sinais, mas também de sua interpretação e configuração de seu significado perante cenários e contextos pré-estabelecidos, e de uma etapa posterior de assimilação do aprendizado.</t>
+  </si>
+  <si>
+    <t>Sinais Fracos - Processo</t>
+  </si>
+  <si>
+    <t>Dessa forma, o processo de captação e processamento de informaçõs, sobretudo os sinais antecipativos, pode ser dividido em três estapas: 1 - a percepção de um estímulo; 2 - a interpretação com a intenção de criar sentido; e 3 - aprendizado ou incorporação de nova informação na representação existente. E uma etapa crítica é a própria definição de relvância do sinal antecipativo observado, principalmente em situação de tempo limitado e excesso de informações, transformando a identificação do sinal fraco em uma função da sensibilidade e do conhecimento do observador.</t>
+  </si>
+  <si>
+    <t>Ademais, a limitação da atividade de inteligência competitiva, na interpretação de sinais fracos, reside na incerteza e complexidade, que afetam o julgamento de seleção da informação, podendo até, em certos casos, ocorrer a criação de filtros simplirficativos e o descarte de informações relevantes.</t>
+  </si>
+  <si>
+    <t>Sinais Fracos - Inteligência Competitiva</t>
+  </si>
+  <si>
+    <t>Verifica-se que, teoricamente, o contexto onde se utiliza a captação e interpretação de sinais fracos, pode muito bem ser utilizado conjuntamente com a identificação de ameaças ou oportunidades estratégicas para a tomada de decisão não rotineira, sugerindo uma possível sinergia de resultados, associada com uma redução na alocação de recursos.</t>
+  </si>
+  <si>
+    <t>A natureza qualitativa e ambígua associada aos sinais fracos, faz com que sua introdução no ambiente corporativo esteja diretamente ligada à capacidade cognitiva das pessoas, para absorver e interpretar as diferentes fontes de informação a que elas se expõem em suas atividades no dia a dia.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinais Fracos </t>
+  </si>
+  <si>
+    <t>Neste sentido, para que um sinal possa vir a ser tratado, é necessário, primeiramente, que alguém o identifique como relevante, e tome a iniciativa de "alertar" a corporação, através de quaisquer meios formais ou informais disponíveis.</t>
+  </si>
+  <si>
+    <t>A identificação de um sinal caracterizado com possível de predizer a ruptura em relação a uma situação estável do ambiente corporativo, pode ser dificultada por fenômenos como o Groupthinking. Neste contexto as pessoas tendem a preferir ignorar um alerta a perturbar o estado de consenso do grupo, ou da organização.</t>
+  </si>
+  <si>
+    <t>Sinais Fracos - Dificuldades</t>
+  </si>
+  <si>
+    <t>Formas de tentar impedir que a organização seja influenciada pelos vieses organizacionais, além da disseminação de uma cultura de encorajamento para a promoção de discussão e pontos de vista conflitantes, também podem ser proporcionadas pela utilização de ferramentas que busquem minimizar as influências sociais do grupo sobre a opinião individual, como por exemplo, utilização de brainstorming (Osborn, 1963) sem a identiciação dos contribuintes, ou a utilização do método Delphi (Linstone &amp; Turoff, 2002).</t>
+  </si>
+  <si>
+    <t>Como resultado secundário, e melhor apresentado adiante, observa-se o aumento da aprendizagem organizacional uma vez o processo e interpretação do sinal fraco, bem como os processos de entendimento e ajustes para a tomada de decisão, demandam a criação coletiva de sentido sobre as informações tratadas, proporcionando a criação de modelos de análise baseados na experiência, bem como formando padrões de tratmento de informações, selleção de alternativas, e decisões, baseadas no conhecimento adquirido.</t>
+  </si>
+  <si>
+    <t>S inais Fracos - Processo - Ganhos</t>
+  </si>
+  <si>
+    <t>A área de inteligência competitiva possui uma natural proximidade com o aprendizado orgnanizacional e a gestão de informação e conhecimento. Isso porque o tratamento contínuo com informação e, sobreturo, a necesidade de filtrar a informação relevante, dentro de uma vasta quantidade disponível, faz com que as áreas afetas à observação do ambiente, e tratamento de ifnormação, possuam mecanismos, ainda que informais, para otimização de suas atividades.</t>
+  </si>
+  <si>
+    <t>A aprendizagem organizacional deve encarregar-se utilizar as experiências passadas, para contribuir, construtivamente, com novas observações e interpretações futuras.</t>
+  </si>
+  <si>
+    <t>Sinais Fracos - Aprendizagem Organizacional</t>
+  </si>
+  <si>
+    <t>Ou seja, verifica-se que existe uma estreita relação entre o aprendizado adquirido na observação de sinais fracos, que demanda um processo estabelecido, regras, condições de observação e valoração de importância da informação, combinação de informações, criação de sentido e proposição de cenários e alternativas; com um processo de gestão de informação e conhecimento empresarial, que dá subsídio à tomada de decisão mais estruturada, fugindo da conotação plítica, incertezas sobre alternativas ambíguas, interferências de vieses pessoais, e influências organizacionais.</t>
+  </si>
+  <si>
+    <t>Sob uma análise mais detida, identificamos que o tratamento de sinais fracos e o processo de tomada de decisão, possuem muitas similaridades: ambos podem ser informais e tratados de forma desconexa, mas estudos apontam que uma maior estruturação de ambas as atividades proporcionam resultados melhores.</t>
+  </si>
+  <si>
+    <t>Conclui-se, portanto, que uma tendência ao estabelecimento de processos formais, tanto para o tratamento de sinais fracos, como a para estruturação da tomada de decisão, vem sendo consolidade, e que a utilização concomitante de esforços de melhoria de desemepnho de ambos podem ser aplicadas, reduzindo, teoricamente, recursos de tempo de investimentos, se consideradas as aplicações de forma distinta.</t>
   </si>
 </sst>
 </file>
@@ -1111,10 +1195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J85"/>
+  <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1164,7 +1248,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1186,7 +1270,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1204,7 +1288,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1225,7 +1309,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1246,7 +1330,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1279,7 +1363,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
@@ -1297,7 +1381,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1315,7 +1399,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>29</v>
       </c>
@@ -1333,7 +1417,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
@@ -1351,7 +1435,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="102" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -1375,7 +1459,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
@@ -1393,7 +1477,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
@@ -1425,7 +1509,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
@@ -1442,7 +1526,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
@@ -1459,7 +1543,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="51" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
@@ -1476,7 +1560,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -1493,7 +1577,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="51" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>47</v>
       </c>
@@ -1510,7 +1594,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>46</v>
       </c>
@@ -1583,7 +1667,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>66</v>
       </c>
@@ -1600,7 +1684,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>68</v>
       </c>
@@ -1617,7 +1701,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>70</v>
       </c>
@@ -1634,7 +1718,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>73</v>
       </c>
@@ -1651,7 +1735,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>77</v>
       </c>
@@ -1668,7 +1752,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>78</v>
       </c>
@@ -1685,7 +1769,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="204" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" ht="191.25" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>81</v>
       </c>
@@ -1693,7 +1777,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="102" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>84</v>
       </c>
@@ -1730,7 +1814,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="C35" s="4" t="s">
         <v>107</v>
       </c>
@@ -1758,7 +1842,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>113</v>
       </c>
@@ -1794,7 +1878,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
     </row>
-    <row r="39" spans="1:10" s="9" customFormat="1" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" s="9" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
@@ -1811,7 +1895,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
     </row>
-    <row r="40" spans="1:10" s="9" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
@@ -1826,12 +1910,12 @@
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
     </row>
-    <row r="41" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D41" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D42" s="2" t="s">
         <v>121</v>
       </c>
@@ -1842,7 +1926,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="102" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="D43" s="2" t="s">
         <v>122</v>
       </c>
@@ -1853,7 +1937,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D44" s="2" t="s">
         <v>124</v>
       </c>
@@ -1864,7 +1948,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="102" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="D45" s="2" t="s">
         <v>125</v>
       </c>
@@ -1875,7 +1959,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D46" s="2" t="s">
         <v>127</v>
       </c>
@@ -1886,7 +1970,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D47" s="2" t="s">
         <v>128</v>
       </c>
@@ -1897,7 +1981,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D48" s="2" t="s">
         <v>129</v>
       </c>
@@ -1908,7 +1992,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="4:8" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D49" s="2" t="s">
         <v>131</v>
       </c>
@@ -1919,7 +2003,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="50" spans="4:8" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D50" s="2" t="s">
         <v>133</v>
       </c>
@@ -1930,7 +2014,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="51" spans="4:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D51" s="2" t="s">
         <v>136</v>
       </c>
@@ -1941,7 +2025,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="4:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D52" s="2" t="s">
         <v>137</v>
       </c>
@@ -1952,7 +2036,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="4:8" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="D53" s="2" t="s">
         <v>138</v>
       </c>
@@ -1963,7 +2047,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="54" spans="4:8" ht="369.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:8" ht="191.25" x14ac:dyDescent="0.25">
       <c r="D54" s="2" t="s">
         <v>140</v>
       </c>
@@ -1974,7 +2058,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="55" spans="4:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D55" s="2" t="s">
         <v>142</v>
       </c>
@@ -1985,7 +2069,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="56" spans="4:8" ht="153" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="D56" s="2" t="s">
         <v>143</v>
       </c>
@@ -1996,7 +2080,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="57" spans="4:8" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D57" s="2" t="s">
         <v>145</v>
       </c>
@@ -2007,7 +2091,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="4:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D58" s="2" t="s">
         <v>147</v>
       </c>
@@ -2018,7 +2102,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="4:8" ht="102" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:8" ht="51" x14ac:dyDescent="0.25">
       <c r="D59" s="2" t="s">
         <v>148</v>
       </c>
@@ -2029,7 +2113,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="60" spans="4:8" ht="102" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:8" ht="51" x14ac:dyDescent="0.25">
       <c r="D60" s="2" t="s">
         <v>149</v>
       </c>
@@ -2040,7 +2124,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D61" s="2" t="s">
         <v>150</v>
       </c>
@@ -2051,7 +2135,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="62" spans="4:8" ht="306" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:8" ht="191.25" x14ac:dyDescent="0.25">
       <c r="D62" s="2" t="s">
         <v>151</v>
       </c>
@@ -2062,7 +2146,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D63" s="2" t="s">
         <v>152</v>
       </c>
@@ -2073,7 +2157,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="64" spans="4:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D64" s="2" t="s">
         <v>153</v>
       </c>
@@ -2084,7 +2168,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="4:8" ht="204" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:8" ht="127.5" x14ac:dyDescent="0.25">
       <c r="D65" s="2" t="s">
         <v>155</v>
       </c>
@@ -2095,7 +2179,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="66" spans="4:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D66" s="2" t="s">
         <v>156</v>
       </c>
@@ -2106,7 +2190,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="4:8" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D67" s="2" t="s">
         <v>157</v>
       </c>
@@ -2260,7 +2344,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="81" spans="4:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="D81" s="2" t="s">
         <v>177</v>
       </c>
@@ -2271,7 +2355,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="82" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D82" s="2" t="s">
         <v>179</v>
       </c>
@@ -2282,7 +2366,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="83" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D83" s="2" t="s">
         <v>180</v>
       </c>
@@ -2293,7 +2377,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="84" spans="4:8" ht="165.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="165.75" x14ac:dyDescent="0.25">
       <c r="D84" s="2" t="s">
         <v>181</v>
       </c>
@@ -2304,7 +2388,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="85" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D85" s="2" t="s">
         <v>182</v>
       </c>
@@ -2313,6 +2397,177 @@
       </c>
       <c r="H85" s="5" t="s">
         <v>183</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H86" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="D87" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G87" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H87" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="D88" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="D89" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G89" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H89" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="D90" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G90" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H90" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="D91" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G91" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="H91" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="D92" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G92" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H92" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="D93" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G93" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="H93" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="D94" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G94" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H94" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="D95" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G95" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H95" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+      <c r="D96" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G96" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H96" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="97" spans="4:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="D97" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G97" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H97" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="98" spans="4:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="D98" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="G98" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="H98" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="99" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="D99" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="G99" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="H99" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="100" spans="4:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="D100" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G100" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H100" s="5" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de referência bibliográfica
</commit_message>
<xml_diff>
--- a/FICHAMENTO.xlsx
+++ b/FICHAMENTO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\weak_signals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C2B56D-191C-452A-8F98-B41FC6040435}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20513CFC-D054-41E5-8784-BE7A8A6A32E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6375" yWindow="2310" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -709,7 +709,79 @@
     <t>No que diz respeito à elaboração de cenários prospectivos, vários autores, como Schwartz, Stffels e Wack, atribuem grande peso às fontes informais, pois estas possuem uma ligação maior com o futuro. Schwartz afirma que nessas fontes é que encontramos os sinais fracos que portam o futuro. O autor sugere que se mantenha contato com "notáveis", pensadores não convencionais, escritores e artistas em geral, porque essas pessoas extrapolam os especialistas e possuem uma visão mais holística e menos quantitativa do mundo.</t>
   </si>
   <si>
-    <t>@article{FonsecaEtAl2012,
+    <t>Processo decisório e o tratamento de sinais fracos</t>
+  </si>
+  <si>
+    <t>Sinais Fracos</t>
+  </si>
+  <si>
+    <t>Sinais Fracos - Motivações</t>
+  </si>
+  <si>
+    <t>Um dos motivos da pouca difusão de práticas de monitoramento do ambiente para identificação e tratamento dos sinais fracos consiste no fato de que a natureza desta atividade se distancia das atividades foco do dia a dia dos gestores.</t>
+  </si>
+  <si>
+    <t>A informação coletada no ambiente, entendida como sinais fracos, é antecipatória, qualitativa, ambígua, fragmentada, pode vir em vários formatos e de várias fontes distrintas (...). Por esse motivo, a conceituação de sinais fracos prescinde de uma estrutura formal, ou de um processo estrabelecido, onde não basta somente a captação dos sinais, mas também de sua interpretação e configuração de seu significado perante cenários e contextos pré-estabelecidos, e de uma etapa posterior de assimilação do aprendizado.</t>
+  </si>
+  <si>
+    <t>Sinais Fracos - Processo</t>
+  </si>
+  <si>
+    <t>Dessa forma, o processo de captação e processamento de informaçõs, sobretudo os sinais antecipativos, pode ser dividido em três estapas: 1 - a percepção de um estímulo; 2 - a interpretação com a intenção de criar sentido; e 3 - aprendizado ou incorporação de nova informação na representação existente. E uma etapa crítica é a própria definição de relvância do sinal antecipativo observado, principalmente em situação de tempo limitado e excesso de informações, transformando a identificação do sinal fraco em uma função da sensibilidade e do conhecimento do observador.</t>
+  </si>
+  <si>
+    <t>Ademais, a limitação da atividade de inteligência competitiva, na interpretação de sinais fracos, reside na incerteza e complexidade, que afetam o julgamento de seleção da informação, podendo até, em certos casos, ocorrer a criação de filtros simplirficativos e o descarte de informações relevantes.</t>
+  </si>
+  <si>
+    <t>Sinais Fracos - Inteligência Competitiva</t>
+  </si>
+  <si>
+    <t>Verifica-se que, teoricamente, o contexto onde se utiliza a captação e interpretação de sinais fracos, pode muito bem ser utilizado conjuntamente com a identificação de ameaças ou oportunidades estratégicas para a tomada de decisão não rotineira, sugerindo uma possível sinergia de resultados, associada com uma redução na alocação de recursos.</t>
+  </si>
+  <si>
+    <t>A natureza qualitativa e ambígua associada aos sinais fracos, faz com que sua introdução no ambiente corporativo esteja diretamente ligada à capacidade cognitiva das pessoas, para absorver e interpretar as diferentes fontes de informação a que elas se expõem em suas atividades no dia a dia.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinais Fracos </t>
+  </si>
+  <si>
+    <t>Neste sentido, para que um sinal possa vir a ser tratado, é necessário, primeiramente, que alguém o identifique como relevante, e tome a iniciativa de "alertar" a corporação, através de quaisquer meios formais ou informais disponíveis.</t>
+  </si>
+  <si>
+    <t>A identificação de um sinal caracterizado com possível de predizer a ruptura em relação a uma situação estável do ambiente corporativo, pode ser dificultada por fenômenos como o Groupthinking. Neste contexto as pessoas tendem a preferir ignorar um alerta a perturbar o estado de consenso do grupo, ou da organização.</t>
+  </si>
+  <si>
+    <t>Sinais Fracos - Dificuldades</t>
+  </si>
+  <si>
+    <t>Formas de tentar impedir que a organização seja influenciada pelos vieses organizacionais, além da disseminação de uma cultura de encorajamento para a promoção de discussão e pontos de vista conflitantes, também podem ser proporcionadas pela utilização de ferramentas que busquem minimizar as influências sociais do grupo sobre a opinião individual, como por exemplo, utilização de brainstorming (Osborn, 1963) sem a identiciação dos contribuintes, ou a utilização do método Delphi (Linstone &amp; Turoff, 2002).</t>
+  </si>
+  <si>
+    <t>Como resultado secundário, e melhor apresentado adiante, observa-se o aumento da aprendizagem organizacional uma vez o processo e interpretação do sinal fraco, bem como os processos de entendimento e ajustes para a tomada de decisão, demandam a criação coletiva de sentido sobre as informações tratadas, proporcionando a criação de modelos de análise baseados na experiência, bem como formando padrões de tratmento de informações, selleção de alternativas, e decisões, baseadas no conhecimento adquirido.</t>
+  </si>
+  <si>
+    <t>S inais Fracos - Processo - Ganhos</t>
+  </si>
+  <si>
+    <t>A área de inteligência competitiva possui uma natural proximidade com o aprendizado orgnanizacional e a gestão de informação e conhecimento. Isso porque o tratamento contínuo com informação e, sobreturo, a necesidade de filtrar a informação relevante, dentro de uma vasta quantidade disponível, faz com que as áreas afetas à observação do ambiente, e tratamento de ifnormação, possuam mecanismos, ainda que informais, para otimização de suas atividades.</t>
+  </si>
+  <si>
+    <t>A aprendizagem organizacional deve encarregar-se utilizar as experiências passadas, para contribuir, construtivamente, com novas observações e interpretações futuras.</t>
+  </si>
+  <si>
+    <t>Sinais Fracos - Aprendizagem Organizacional</t>
+  </si>
+  <si>
+    <t>Ou seja, verifica-se que existe uma estreita relação entre o aprendizado adquirido na observação de sinais fracos, que demanda um processo estabelecido, regras, condições de observação e valoração de importância da informação, combinação de informações, criação de sentido e proposição de cenários e alternativas; com um processo de gestão de informação e conhecimento empresarial, que dá subsídio à tomada de decisão mais estruturada, fugindo da conotação plítica, incertezas sobre alternativas ambíguas, interferências de vieses pessoais, e influências organizacionais.</t>
+  </si>
+  <si>
+    <t>Sob uma análise mais detida, identificamos que o tratamento de sinais fracos e o processo de tomada de decisão, possuem muitas similaridades: ambos podem ser informais e tratados de forma desconexa, mas estudos apontam que uma maior estruturação de ambas as atividades proporcionam resultados melhores.</t>
+  </si>
+  <si>
+    <t>Conclui-se, portanto, que uma tendência ao estabelecimento de processos formais, tanto para o tratamento de sinais fracos, como a para estruturação da tomada de decisão, vem sendo consolidade, e que a utilização concomitante de esforços de melhoria de desemepnho de ambos podem ser aplicadas, reduzindo, teoricamente, recursos de tempo de investimentos, se consideradas as aplicações de forma distinta.</t>
+  </si>
+  <si>
+    <t>@article{FonsecaBarretoEtAl2012,
 author = {Fonseca, Fernando and Mello Barreto, Luis Fernando},
 year = {2012},
 month = {01},
@@ -719,78 +791,6 @@
 journal = {Future Studies Research Journal: Trends and Strategies},
 doi = {10.24023/FutureJournal/2175-5825/2011.v3i2.80}
 }</t>
-  </si>
-  <si>
-    <t>Processo decisório e o tratamento de sinais fracos</t>
-  </si>
-  <si>
-    <t>Sinais Fracos</t>
-  </si>
-  <si>
-    <t>Sinais Fracos - Motivações</t>
-  </si>
-  <si>
-    <t>Um dos motivos da pouca difusão de práticas de monitoramento do ambiente para identificação e tratamento dos sinais fracos consiste no fato de que a natureza desta atividade se distancia das atividades foco do dia a dia dos gestores.</t>
-  </si>
-  <si>
-    <t>A informação coletada no ambiente, entendida como sinais fracos, é antecipatória, qualitativa, ambígua, fragmentada, pode vir em vários formatos e de várias fontes distrintas (...). Por esse motivo, a conceituação de sinais fracos prescinde de uma estrutura formal, ou de um processo estrabelecido, onde não basta somente a captação dos sinais, mas também de sua interpretação e configuração de seu significado perante cenários e contextos pré-estabelecidos, e de uma etapa posterior de assimilação do aprendizado.</t>
-  </si>
-  <si>
-    <t>Sinais Fracos - Processo</t>
-  </si>
-  <si>
-    <t>Dessa forma, o processo de captação e processamento de informaçõs, sobretudo os sinais antecipativos, pode ser dividido em três estapas: 1 - a percepção de um estímulo; 2 - a interpretação com a intenção de criar sentido; e 3 - aprendizado ou incorporação de nova informação na representação existente. E uma etapa crítica é a própria definição de relvância do sinal antecipativo observado, principalmente em situação de tempo limitado e excesso de informações, transformando a identificação do sinal fraco em uma função da sensibilidade e do conhecimento do observador.</t>
-  </si>
-  <si>
-    <t>Ademais, a limitação da atividade de inteligência competitiva, na interpretação de sinais fracos, reside na incerteza e complexidade, que afetam o julgamento de seleção da informação, podendo até, em certos casos, ocorrer a criação de filtros simplirficativos e o descarte de informações relevantes.</t>
-  </si>
-  <si>
-    <t>Sinais Fracos - Inteligência Competitiva</t>
-  </si>
-  <si>
-    <t>Verifica-se que, teoricamente, o contexto onde se utiliza a captação e interpretação de sinais fracos, pode muito bem ser utilizado conjuntamente com a identificação de ameaças ou oportunidades estratégicas para a tomada de decisão não rotineira, sugerindo uma possível sinergia de resultados, associada com uma redução na alocação de recursos.</t>
-  </si>
-  <si>
-    <t>A natureza qualitativa e ambígua associada aos sinais fracos, faz com que sua introdução no ambiente corporativo esteja diretamente ligada à capacidade cognitiva das pessoas, para absorver e interpretar as diferentes fontes de informação a que elas se expõem em suas atividades no dia a dia.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sinais Fracos </t>
-  </si>
-  <si>
-    <t>Neste sentido, para que um sinal possa vir a ser tratado, é necessário, primeiramente, que alguém o identifique como relevante, e tome a iniciativa de "alertar" a corporação, através de quaisquer meios formais ou informais disponíveis.</t>
-  </si>
-  <si>
-    <t>A identificação de um sinal caracterizado com possível de predizer a ruptura em relação a uma situação estável do ambiente corporativo, pode ser dificultada por fenômenos como o Groupthinking. Neste contexto as pessoas tendem a preferir ignorar um alerta a perturbar o estado de consenso do grupo, ou da organização.</t>
-  </si>
-  <si>
-    <t>Sinais Fracos - Dificuldades</t>
-  </si>
-  <si>
-    <t>Formas de tentar impedir que a organização seja influenciada pelos vieses organizacionais, além da disseminação de uma cultura de encorajamento para a promoção de discussão e pontos de vista conflitantes, também podem ser proporcionadas pela utilização de ferramentas que busquem minimizar as influências sociais do grupo sobre a opinião individual, como por exemplo, utilização de brainstorming (Osborn, 1963) sem a identiciação dos contribuintes, ou a utilização do método Delphi (Linstone &amp; Turoff, 2002).</t>
-  </si>
-  <si>
-    <t>Como resultado secundário, e melhor apresentado adiante, observa-se o aumento da aprendizagem organizacional uma vez o processo e interpretação do sinal fraco, bem como os processos de entendimento e ajustes para a tomada de decisão, demandam a criação coletiva de sentido sobre as informações tratadas, proporcionando a criação de modelos de análise baseados na experiência, bem como formando padrões de tratmento de informações, selleção de alternativas, e decisões, baseadas no conhecimento adquirido.</t>
-  </si>
-  <si>
-    <t>S inais Fracos - Processo - Ganhos</t>
-  </si>
-  <si>
-    <t>A área de inteligência competitiva possui uma natural proximidade com o aprendizado orgnanizacional e a gestão de informação e conhecimento. Isso porque o tratamento contínuo com informação e, sobreturo, a necesidade de filtrar a informação relevante, dentro de uma vasta quantidade disponível, faz com que as áreas afetas à observação do ambiente, e tratamento de ifnormação, possuam mecanismos, ainda que informais, para otimização de suas atividades.</t>
-  </si>
-  <si>
-    <t>A aprendizagem organizacional deve encarregar-se utilizar as experiências passadas, para contribuir, construtivamente, com novas observações e interpretações futuras.</t>
-  </si>
-  <si>
-    <t>Sinais Fracos - Aprendizagem Organizacional</t>
-  </si>
-  <si>
-    <t>Ou seja, verifica-se que existe uma estreita relação entre o aprendizado adquirido na observação de sinais fracos, que demanda um processo estabelecido, regras, condições de observação e valoração de importância da informação, combinação de informações, criação de sentido e proposição de cenários e alternativas; com um processo de gestão de informação e conhecimento empresarial, que dá subsídio à tomada de decisão mais estruturada, fugindo da conotação plítica, incertezas sobre alternativas ambíguas, interferências de vieses pessoais, e influências organizacionais.</t>
-  </si>
-  <si>
-    <t>Sob uma análise mais detida, identificamos que o tratamento de sinais fracos e o processo de tomada de decisão, possuem muitas similaridades: ambos podem ser informais e tratados de forma desconexa, mas estudos apontam que uma maior estruturação de ambas as atividades proporcionam resultados melhores.</t>
-  </si>
-  <si>
-    <t>Conclui-se, portanto, que uma tendência ao estabelecimento de processos formais, tanto para o tratamento de sinais fracos, como a para estruturação da tomada de decisão, vem sendo consolidade, e que a utilização concomitante de esforços de melhoria de desemepnho de ambos podem ser aplicadas, reduzindo, teoricamente, recursos de tempo de investimentos, se consideradas as aplicações de forma distinta.</t>
   </si>
 </sst>
 </file>
@@ -1197,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView tabSelected="1" topLeftCell="E85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I86" sqref="I86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2401,71 +2401,71 @@
     </row>
     <row r="86" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G86" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="D86" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G86" s="6" t="s">
+      <c r="H86" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="H86" s="5" t="s">
-        <v>188</v>
-      </c>
       <c r="I86" s="4" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="D87" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G87" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="H87" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="G87" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="H87" s="5" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="D88" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H88" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D89" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="G89" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="H89" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="G89" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="H89" s="5" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D90" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H90" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D91" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G91" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="G91" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="H91" s="5" t="s">
         <v>144</v>
@@ -2473,10 +2473,10 @@
     </row>
     <row r="92" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D92" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H92" s="5" t="s">
         <v>144</v>
@@ -2484,90 +2484,90 @@
     </row>
     <row r="93" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D93" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G93" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="H93" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="G93" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="H93" s="5" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="D94" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H94" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="D95" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G95" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="H95" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="G95" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="H95" s="5" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="D96" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H96" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="97" spans="4:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D97" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G97" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="H97" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="G97" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="H97" s="5" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="98" spans="4:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="D98" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H98" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="99" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D99" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H99" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="100" spans="4:8" ht="51" x14ac:dyDescent="0.25">
       <c r="D100" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H100" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inclusão de artigos da pesquisa e alterações na estrutura da dissertação
</commit_message>
<xml_diff>
--- a/FICHAMENTO.xlsx
+++ b/FICHAMENTO.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigosantos/Documents/GitHub/weak_signals/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\weak_signals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A303C0B8-35D3-4246-A4F0-3AB66626A82E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54689366-DE9B-421E-B678-4DC14D18ED27}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="1020" windowWidth="16155" windowHeight="13200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$J$84</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="262">
   <si>
     <t>Título</t>
   </si>
@@ -803,12 +804,171 @@
   publisher={Editora FGV}
 }</t>
   </si>
+  <si>
+    <t>@inproceedings{inproceedings,
+author = {Freitas, Henrique and Janissek-Muniz, Raquel},
+year = {2006},
+month = {01},
+pages = {},
+title = {Uma proposta de plataforma para Inteligência Estratégica}
+}</t>
+  </si>
+  <si>
+    <t>Uma proposta de plataforma para inteligência estratégica</t>
+  </si>
+  <si>
+    <t>Em outras formas para melhor se definir a gestão de informação, tem-se a abordagem do planejamento estratégico (missão, objetivos, fatores críticos etc) e a do processo decisório (inteligência, concepção, escolha, revisão). A abordagem de inteligência estratégica que se pretende desenvolver vem se agregar a esses modelos, no intuito de antecipação de problemas e de identificação de oportunidades, a partir de uma maior e especial atenção aos ambientes internos (capacidades e limites), externo (ameaças e oportunidades) e social (oi ambiente maior no qual se insere a organização).</t>
+  </si>
+  <si>
+    <t>Inteligência estratégica</t>
+  </si>
+  <si>
+    <t>Utilização</t>
+  </si>
+  <si>
+    <t>Para tal, é necessário que se encontrem meios de reunir e potencializar o uso de sistemas de informação que integrem conceitos de gestão, métodos, modlos estatísticos, técnicas de análises de textos, tecnologia Web, tudo isso, para que a energia principal da atividade se concentre na efetiva exploreação, análise, interpretação de dados.</t>
+  </si>
+  <si>
+    <t>Sistema de informação</t>
+  </si>
+  <si>
+    <t>Os métodos, técnicas e ferramental existente nem sempre respondem às características de implantação de um processo de inteligência, pois nem sempre permitem a gestão de informação informal, pouco estruturada, aleatória e essencialmente indeterminada.</t>
+  </si>
+  <si>
+    <t>A pertinência de uma informação é definida a partir de uma série de critérios ou características que farão com que uma determinada informação seja útil. E assim um paradoxo se estabelece: pouca ou muita informação? O que privilegiar? Como encontrar? Como selecionar aquelas de fato pertinentes?</t>
+  </si>
+  <si>
+    <t>Seleção de informações importantes</t>
+  </si>
+  <si>
+    <t>Enfim, mais do que quantidade, é necessário rapidez, seletividade e qualidade na informação, que precisa ser coletada, armazenada, processada e difundida. Deve-se zelar para que a informação produzida nesse processo todo seja atual, correta, confiável e de fácil compreensão.</t>
+  </si>
+  <si>
+    <t>Informação produzida</t>
+  </si>
+  <si>
+    <t>Já não existe mais o problema de acesso aos dados (vide a internet, qu representa por si só uma fonte inesgotável): o grande desafio que hoje confrontamos é a produção de conhecimento através das informações.</t>
+  </si>
+  <si>
+    <t>Acesso a dados</t>
+  </si>
+  <si>
+    <t>Muitas vezes é necessário, no dia-a-dia, justificar de maneira mais formal decisões que se norteiam principalmente pelo bom senso, isto melhor convencendo àqueles que preferem dados analisados e apresentados com maior estruturação ou que não dispõem de um corpo técnico capacitado para a análise destes dados.</t>
+  </si>
+  <si>
+    <t>Além da busca pela informação, existe o aspecto de seleção e julgamento, num primeiro momento individual, e posteriormente coletivo, que deve ser organizado e de certa forma gerenciado.</t>
+  </si>
+  <si>
+    <t>Seleção e julgamento de dados</t>
+  </si>
+  <si>
+    <t>Ao tratar a questão da informação, diversos itens devem ser considerados: Que tipo de informação? Qual informação? Informação para quem? Informação obtida onde? Por que "esta" informação? Informação obtida como? Informação obtida quando? Informação entregue quando? Informação para fazer o que? Informação para decisão, ou decisão pela informação?</t>
+  </si>
+  <si>
+    <t>O problema do tomador de decisão e do papel da TI envolvido neste processo é justamente adequar a forma, o foco e o meio de obtenção ao tipo e à qual informação específica observar, zelando sempre pela pertinência dos dados coletados através de métodos determinados e, uma vez produzida a informação, decidir igualmente o quê, como e a quem comunicar.</t>
+  </si>
+  <si>
+    <t>Aquisição da informação</t>
+  </si>
+  <si>
+    <t>A orgnaização da informação para tomada de decisão sempre visa a antecipação de problemas e a identificação de oportunidades, bem como a definição de estratégias para melhor aproveitar essas oportunidades. Dois elementos principais servirão de fonte fundamental: a própria organização (com a identificação de forças e capacidades e limitações e fraquezas, e com coleta em diferentes etapas de cada processo, pré-transação e pós-transação), que é por definição controlável, e o ambiente no qual se insere a organização (as leis, opolítica, economia, concorrência, mercado, fornecedores, tecnologia etc) o qual é pressuportamente incontrolável, contudo deve-se necesssariamente procurar, no mínimo, monitorá-lo. Isto é o que define o escopo de um mecanismo ou sistema de inteligência organizacional, o que vamos mais adiante desenvolver.</t>
+  </si>
+  <si>
+    <t>Organização da informação</t>
+  </si>
+  <si>
+    <t>É necessário valorizar todo sistema de informação com suas ramificações e fontes quantitativas e qualitativas, ou seja, deve-se explorar os dados para encontrar os bons filões. Com os dados bem estruturados, vamos provavalmente identificar mais rapidamente as informações úteis. Já com os dados mais heterogêneos, menos estruturados, mais qualitativos, onde certamente há bons filões a identificar, deve haver trodo um esforço de análise e interpretação.</t>
+  </si>
+  <si>
+    <t>Há diversas dimensões segundo as quais se pode categorizar os dados coletados: Formal x Informal, Quantitativa x Qualitativa, Interna x Externa, Disponível x Indisponível, Retrospectiva x Antecipativa x Atual, Aleatória x Não aleatória, Ambígua x Não ambígua, Familiar x Não familiar, Confiável x Não confiável, Fragmentada  x Não fragmentada, Completa x Incompleta, Operacional x Estratégica, Fatual x Subjetiva, Verbal x Escrita x Visual x Olfativa x Táctil, Visísl x Não visível.</t>
+  </si>
+  <si>
+    <t>Categorias de informação</t>
+  </si>
+  <si>
+    <t>Não basta uma informação possuir qualidades suficientes para ser considerada pertinente se esta não puder ser acessada no momento desejado. De fato, tão importante quanto as características de uma informação são as fontes onde esta pode ser obtida e as formas ou possibilidades de acesso às mesmas.</t>
+  </si>
+  <si>
+    <t>Muitas vezes, é a própria fonte de informação que influencia diretaemtne na característica de uma informação. Por exemplo, em função da fonte onde ela foi obtida, uma informação pode ou não ser confiável.</t>
+  </si>
+  <si>
+    <t>Fonte de informação</t>
+  </si>
+  <si>
+    <t>Exemplos de fontes de informação podem ser: internet, bases de dados internas ou externas, fornecedores, clientes, revistas, jornais, períodicos, congressos, seminários, feiras, exposições, publicações científicas e técnicas, registros de marcas e patentes, teses, dissertações, projetos e publicações de pesquisas, publicações da organização (relatório anual, por exemplo), tribunais de comércio, produtos de concorrentes, missões e viagens de estudo, contatos pessoais, ofertas de emprego, negociações comerciais, bolsa de valores, livros e enciblopédias, relatórios de serviços e missões oficiais, relatórios e sínteses de empresas especializadas na coleta de informações.</t>
+  </si>
+  <si>
+    <t>Globalmente, uma informação é tanto mais importante ou valorizada quanto maior for sua contribuição ao processo decisório. O valor da informação é dificil ou complexo de ser medido ou observado: há aspectos tangíveis, mensuráveis, mas há diversos aspectos intangíveis, reflexos ou efeitos indiretos, os quais são delicados de perceber e apreciar.</t>
+  </si>
+  <si>
+    <t>Valor da informação</t>
+  </si>
+  <si>
+    <t>As atividades de atenção e monitoramento para a identificação de informações pertinentes e úteis à tomada de decisão podem ser suportadas pela implantação de disponsitivos de inteligência que permitam alavancar a compreeensão do ambiente, auxiliando na condução das estratégias organizacionais e no uso otimizado dos recursos disponíveis.</t>
+  </si>
+  <si>
+    <t>A inteligência estratégica parte da premissa que, ao conhecer o ambiente no qual a empresa está inserida, tem-se um incremento importante em relação à estratégia da organização, pois propicia uma adequação e preparação, a tempo, para enfrentar o ambiente turbulento e incerto a que estão submetidas.</t>
+  </si>
+  <si>
+    <t>Características</t>
+  </si>
+  <si>
+    <t>Diversos são os desafios ligados à implantação de um tal projeto na orgranização. Entre eles citamos: sensibilizar a direção para reconhecimento da importância de um projeto de Inteligência; definir uma equipe de projeto engajada e de competências diversas; formar pessoas para coleta, seleção e análise das informações; delimitrar o ambiente prioritário para ação; identificar o tipo de informçaão pertinente para a empresa, a forma adequada de selecioná-las; definir tecnologias de suporte ao processo.</t>
+  </si>
+  <si>
+    <t>Processo implantação inteligencia</t>
+  </si>
+  <si>
+    <t>O principal objetivo da inteligência estratégica é oferecer um suporte simples e eficaz para que através da arquisição e interpretação da informação pertinente se possa melhor conduzir as estratéfgias e utilizar de forma mais eficaz os recursos da organização, melhorando o processo decisório, e assim melhor enfrentando as turbulências do ambiente.</t>
+  </si>
+  <si>
+    <t>Estados de Conhecimento</t>
+  </si>
+  <si>
+    <t>(1) Senso de ameaça/oportunidade</t>
+  </si>
+  <si>
+    <t>(2) Fonte da ameaça/oportunidade</t>
+  </si>
+  <si>
+    <t>(3) Ameaça/Oportunidade Concreta</t>
+  </si>
+  <si>
+    <t>(4) Resposta Concreta</t>
+  </si>
+  <si>
+    <t>(5) Resultado Concreto</t>
+  </si>
+  <si>
+    <t>Informação Conteúdo</t>
+  </si>
+  <si>
+    <t>Convicção de que discontinuidades são iminentes</t>
+  </si>
+  <si>
+    <t>Fonte da discontinuidade identificada</t>
+  </si>
+  <si>
+    <t>Características, natureza, gravidade, e tempo de impacto entendidos</t>
+  </si>
+  <si>
+    <t>Resposta identificada, tempo, ação, programas, oraçamento podem ser identificados</t>
+  </si>
+  <si>
+    <t>Impacto no lucro e consequencias das respostas são computados</t>
+  </si>
+  <si>
+    <t>SIM</t>
+  </si>
+  <si>
+    <t>NÃO</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -839,8 +999,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -850,6 +1022,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -866,7 +1056,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -900,6 +1090,39 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1215,28 +1438,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J100"/>
+  <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B91" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView topLeftCell="D102" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G122" sqref="G122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="91.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="98.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="89.875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="4.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.625" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="233.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="5"/>
+    <col min="8" max="8" width="32.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="233.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1268,7 +1491,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1290,7 +1513,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1308,7 +1531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1329,7 +1552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1350,7 +1573,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="42" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1368,7 +1591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="84" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
@@ -1383,7 +1606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
@@ -1401,7 +1624,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1419,7 +1642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="70" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>29</v>
       </c>
@@ -1437,7 +1660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="70" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
@@ -1455,7 +1678,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="56" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -1479,7 +1702,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
@@ -1497,7 +1720,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="42" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
@@ -1515,7 +1738,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
@@ -1529,7 +1752,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
@@ -1546,7 +1769,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="28" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
@@ -1563,7 +1786,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="56" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" ht="51" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
@@ -1580,7 +1803,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="14" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -1597,7 +1820,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="56" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" ht="51" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>47</v>
       </c>
@@ -1614,7 +1837,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="28" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>46</v>
       </c>
@@ -1631,7 +1854,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>51</v>
       </c>
@@ -1645,7 +1868,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="84" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>53</v>
       </c>
@@ -1659,7 +1882,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="98" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" ht="89.25" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>62</v>
       </c>
@@ -1673,7 +1896,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="112" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" ht="102" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>63</v>
       </c>
@@ -1687,7 +1910,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="28" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>66</v>
       </c>
@@ -1704,7 +1927,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="42" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>68</v>
       </c>
@@ -1721,7 +1944,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="42" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>70</v>
       </c>
@@ -1738,7 +1961,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="56" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>73</v>
       </c>
@@ -1755,7 +1978,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="42" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>77</v>
       </c>
@@ -1772,7 +1995,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="42" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>78</v>
       </c>
@@ -1789,7 +2012,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="224" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" ht="191.25" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>81</v>
       </c>
@@ -1797,7 +2020,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="56" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>84</v>
       </c>
@@ -1814,7 +2037,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="84" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>101</v>
       </c>
@@ -1834,7 +2057,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="42" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="C35" s="4" t="s">
         <v>107</v>
       </c>
@@ -1848,7 +2071,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="42" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D36" s="2" t="s">
         <v>110</v>
       </c>
@@ -1862,7 +2085,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="9" customFormat="1" ht="28" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>113</v>
       </c>
@@ -1883,7 +2106,7 @@
       </c>
       <c r="J37" s="8"/>
     </row>
-    <row r="38" spans="1:10" s="9" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
@@ -1900,7 +2123,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
     </row>
-    <row r="39" spans="1:10" s="9" customFormat="1" ht="70" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" s="9" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
@@ -1917,7 +2140,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
     </row>
-    <row r="40" spans="1:10" s="9" customFormat="1" ht="42" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
@@ -1932,12 +2155,12 @@
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
     </row>
-    <row r="41" spans="1:10" ht="42" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D41" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D42" s="2" t="s">
         <v>121</v>
       </c>
@@ -1948,7 +2171,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="56" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="D43" s="2" t="s">
         <v>122</v>
       </c>
@@ -1959,7 +2182,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D44" s="2" t="s">
         <v>124</v>
       </c>
@@ -1970,7 +2193,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="56" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="D45" s="2" t="s">
         <v>125</v>
       </c>
@@ -1981,7 +2204,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D46" s="2" t="s">
         <v>127</v>
       </c>
@@ -1992,7 +2215,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="28" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D47" s="2" t="s">
         <v>128</v>
       </c>
@@ -2003,7 +2226,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="42" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D48" s="2" t="s">
         <v>129</v>
       </c>
@@ -2014,7 +2237,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="4:8" ht="42" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D49" s="2" t="s">
         <v>131</v>
       </c>
@@ -2025,7 +2248,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="50" spans="4:8" ht="42" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D50" s="2" t="s">
         <v>133</v>
       </c>
@@ -2036,7 +2259,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="51" spans="4:8" ht="28" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D51" s="2" t="s">
         <v>136</v>
       </c>
@@ -2047,7 +2270,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="4:8" ht="42" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D52" s="2" t="s">
         <v>137</v>
       </c>
@@ -2058,7 +2281,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="4:8" ht="84" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="D53" s="2" t="s">
         <v>138</v>
       </c>
@@ -2069,7 +2292,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="54" spans="4:8" ht="238" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:8" ht="229.5" x14ac:dyDescent="0.25">
       <c r="D54" s="2" t="s">
         <v>140</v>
       </c>
@@ -2080,7 +2303,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="55" spans="4:8" ht="28" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D55" s="2" t="s">
         <v>142</v>
       </c>
@@ -2091,7 +2314,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="56" spans="4:8" ht="84" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="D56" s="2" t="s">
         <v>143</v>
       </c>
@@ -2102,7 +2325,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="57" spans="4:8" ht="42" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D57" s="2" t="s">
         <v>145</v>
       </c>
@@ -2113,7 +2336,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="4:8" ht="28" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D58" s="2" t="s">
         <v>147</v>
       </c>
@@ -2124,7 +2347,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="59" spans="4:8" ht="56" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:8" ht="51" x14ac:dyDescent="0.25">
       <c r="D59" s="2" t="s">
         <v>148</v>
       </c>
@@ -2135,7 +2358,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="60" spans="4:8" ht="56" x14ac:dyDescent="0.2">
+    <row r="60" spans="4:8" ht="51" x14ac:dyDescent="0.25">
       <c r="D60" s="2" t="s">
         <v>149</v>
       </c>
@@ -2146,7 +2369,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="4:8" ht="28" x14ac:dyDescent="0.2">
+    <row r="61" spans="4:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D61" s="2" t="s">
         <v>150</v>
       </c>
@@ -2157,7 +2380,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="62" spans="4:8" ht="210" x14ac:dyDescent="0.2">
+    <row r="62" spans="4:8" ht="204" x14ac:dyDescent="0.25">
       <c r="D62" s="2" t="s">
         <v>151</v>
       </c>
@@ -2168,7 +2391,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="63" spans="4:8" ht="28" x14ac:dyDescent="0.2">
+    <row r="63" spans="4:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D63" s="2" t="s">
         <v>152</v>
       </c>
@@ -2179,7 +2402,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="64" spans="4:8" ht="28" x14ac:dyDescent="0.2">
+    <row r="64" spans="4:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D64" s="2" t="s">
         <v>153</v>
       </c>
@@ -2190,7 +2413,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="4:8" ht="140" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:8" ht="127.5" x14ac:dyDescent="0.25">
       <c r="D65" s="2" t="s">
         <v>155</v>
       </c>
@@ -2201,7 +2424,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="66" spans="4:8" ht="42" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D66" s="2" t="s">
         <v>156</v>
       </c>
@@ -2212,7 +2435,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="4:8" ht="42" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:8" ht="51" x14ac:dyDescent="0.25">
       <c r="D67" s="2" t="s">
         <v>157</v>
       </c>
@@ -2223,7 +2446,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="4:8" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="68" spans="4:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="D68" s="2" t="s">
         <v>158</v>
       </c>
@@ -2234,7 +2457,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="69" spans="4:8" ht="70" x14ac:dyDescent="0.2">
+    <row r="69" spans="4:8" ht="76.5" x14ac:dyDescent="0.25">
       <c r="D69" s="2" t="s">
         <v>159</v>
       </c>
@@ -2245,7 +2468,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="70" spans="4:8" ht="28" x14ac:dyDescent="0.2">
+    <row r="70" spans="4:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D70" s="2" t="s">
         <v>161</v>
       </c>
@@ -2256,7 +2479,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="71" spans="4:8" ht="98" x14ac:dyDescent="0.2">
+    <row r="71" spans="4:8" ht="89.25" x14ac:dyDescent="0.25">
       <c r="D71" s="2" t="s">
         <v>162</v>
       </c>
@@ -2267,7 +2490,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="72" spans="4:8" ht="42" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D72" s="2" t="s">
         <v>164</v>
       </c>
@@ -2278,7 +2501,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="73" spans="4:8" ht="28" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D73" s="2" t="s">
         <v>166</v>
       </c>
@@ -2289,7 +2512,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="74" spans="4:8" ht="84" x14ac:dyDescent="0.2">
+    <row r="74" spans="4:8" ht="89.25" x14ac:dyDescent="0.25">
       <c r="D74" s="2" t="s">
         <v>168</v>
       </c>
@@ -2300,7 +2523,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="75" spans="4:8" ht="14" x14ac:dyDescent="0.2">
+    <row r="75" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D75" s="2" t="s">
         <v>169</v>
       </c>
@@ -2311,7 +2534,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="76" spans="4:8" ht="70" x14ac:dyDescent="0.2">
+    <row r="76" spans="4:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="D76" s="2" t="s">
         <v>184</v>
       </c>
@@ -2322,7 +2545,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="77" spans="4:8" ht="28" x14ac:dyDescent="0.2">
+    <row r="77" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D77" s="2" t="s">
         <v>172</v>
       </c>
@@ -2333,7 +2556,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="78" spans="4:8" ht="42" x14ac:dyDescent="0.2">
+    <row r="78" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D78" s="2" t="s">
         <v>174</v>
       </c>
@@ -2344,7 +2567,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="79" spans="4:8" ht="42" x14ac:dyDescent="0.2">
+    <row r="79" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D79" s="2" t="s">
         <v>175</v>
       </c>
@@ -2355,7 +2578,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="80" spans="4:8" ht="56" x14ac:dyDescent="0.2">
+    <row r="80" spans="4:8" ht="51" x14ac:dyDescent="0.25">
       <c r="D80" s="2" t="s">
         <v>176</v>
       </c>
@@ -2366,7 +2589,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="56" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="D81" s="11" t="s">
         <v>177</v>
       </c>
@@ -2377,7 +2600,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="42" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D82" s="2" t="s">
         <v>179</v>
       </c>
@@ -2388,7 +2611,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="42" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D83" s="2" t="s">
         <v>180</v>
       </c>
@@ -2399,7 +2622,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="182" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="178.5" x14ac:dyDescent="0.25">
       <c r="D84" s="2" t="s">
         <v>181</v>
       </c>
@@ -2410,7 +2633,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="42" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D85" s="2" t="s">
         <v>182</v>
       </c>
@@ -2421,7 +2644,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="28" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>185</v>
       </c>
@@ -2438,7 +2661,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="70" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="D87" s="2" t="s">
         <v>189</v>
       </c>
@@ -2449,7 +2672,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="70" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="D88" s="2" t="s">
         <v>191</v>
       </c>
@@ -2460,7 +2683,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="42" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D89" s="2" t="s">
         <v>192</v>
       </c>
@@ -2471,7 +2694,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="42" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D90" s="2" t="s">
         <v>194</v>
       </c>
@@ -2482,7 +2705,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="42" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D91" s="2" t="s">
         <v>195</v>
       </c>
@@ -2493,7 +2716,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="28" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D92" s="2" t="s">
         <v>197</v>
       </c>
@@ -2504,7 +2727,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="42" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D93" s="2" t="s">
         <v>198</v>
       </c>
@@ -2515,7 +2738,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="70" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="D94" s="2" t="s">
         <v>200</v>
       </c>
@@ -2526,7 +2749,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="70" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="D95" s="2" t="s">
         <v>201</v>
       </c>
@@ -2537,7 +2760,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="56" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="D96" s="2" t="s">
         <v>203</v>
       </c>
@@ -2548,7 +2771,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="97" spans="4:8" ht="28" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="D97" s="2" t="s">
         <v>204</v>
       </c>
@@ -2559,7 +2782,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="98" spans="4:8" ht="70" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="D98" s="2" t="s">
         <v>206</v>
       </c>
@@ -2570,7 +2793,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="99" spans="4:8" ht="42" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="D99" s="2" t="s">
         <v>207</v>
       </c>
@@ -2581,7 +2804,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="100" spans="4:8" ht="56" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="D100" s="2" t="s">
         <v>208</v>
       </c>
@@ -2590,11 +2813,413 @@
       </c>
       <c r="H100" s="5" t="s">
         <v>190</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="G101" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H101" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="I101" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="D102" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="G102" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H102" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="D103" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="G103" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H103" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="D104" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G104" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H104" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="D105" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="G105" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H105" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="D106" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G106" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H106" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="D107" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="G107" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H107" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="D108" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G108" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H108" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+      <c r="D109" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G109" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H109" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+      <c r="D110" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G110" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H110" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+      <c r="D111" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="G111" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H111" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+      <c r="D112" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="G112" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H112" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="113" spans="4:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="D113" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="G113" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H113" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="114" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="D114" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="G114" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H114" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="115" spans="4:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="D115" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="G115" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H115" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="116" spans="4:8" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="D116" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G116" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H116" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="117" spans="4:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="D117" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="G117" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H117" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="118" spans="4:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="D118" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="G118" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H118" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="119" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="D119" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G119" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H119" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="120" spans="4:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="D120" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G120" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H120" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="121" spans="4:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="D121" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G121" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H121" s="5" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J84" xr:uid="{7C177F3E-3F7D-4913-AABA-E34D03F168B6}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF29B1F-2193-4DC8-A844-02A61142BFD2}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="27.375" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21.25" style="12" customWidth="1"/>
+    <col min="5" max="5" width="25.625" style="12" customWidth="1"/>
+    <col min="6" max="7" width="21.25" style="12" customWidth="1"/>
+    <col min="8" max="16384" width="13.5" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+    </row>
+    <row r="2" spans="1:7" s="14" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>260</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="A3:A7"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Terminada mais uma leitura para embasamento teórico e atualização do fichamento
</commit_message>
<xml_diff>
--- a/FICHAMENTO.xlsx
+++ b/FICHAMENTO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\weak_signals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigosantos/Documents/GitHub/weak_signals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5761E1CA-3E23-4A0D-9075-B14A2487B4FD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053CAD05-14E6-954B-B737-CEFC871C6519}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="1620" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5000" yWindow="-21140" windowWidth="38260" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$J$84</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="349">
   <si>
     <t>Título</t>
   </si>
@@ -1096,6 +1095,167 @@
   author={Godet, Michel and Roubelat, Fabrice},
   year={1996}
 }</t>
+  </si>
+  <si>
+    <t>To transform anticipation into action through appropriation, scenarios should follow four conditions: relvance, consistence, likelihood and transparency.</t>
+  </si>
+  <si>
+    <t>If the future were totally foreseeable and certain, the present would become unliveable.</t>
+  </si>
+  <si>
+    <t>Although the world is changing, the direction of this change is uncertain. La prospective does not claim to eliminate this uncertainty through illusory prediction, but aims to reduce it as far as possible,  and to make decisionsbased as little as possible on hypothetical futures. Thus, the first aim of La prospective is to illuminate the choices of the present in the light of possible futures. Good forecasts are not necesssarily those which are realised, but those which lead to action so as to avoid the dangers and arrive at the desired objective.</t>
+  </si>
+  <si>
+    <t>Over the last two decades we have also notived that errors of forecasting area often based upon two mistakes: overestimation of the pace of change (of technologies); underestimation of inertial factors (structures, behaviours). Therefore, when thinking about the future, we suggest it is useful to start by identifying factors which area unlikely to change.</t>
+  </si>
+  <si>
+    <t>Differing from forecasting which is too often coined with econometrics, foresight which remains too passive, futures studies which is too large, strategic prospective is not only na exploratory approach but also a normative one. Cotinuing the tradition of strategic planning and strategic management, strategic prospective emphasizes the importance of long range and alternative thinking in strategic decision processes.</t>
+  </si>
+  <si>
+    <t>Any thinking which is not appropriated by those concerned has a great chance to be rejected. Thus we discover the three components of the Greek trianlge: prospective thought gi er content to mobilisation, maintains motivation (ie: motives for action) and nourishes strategic will)</t>
+  </si>
+  <si>
+    <t>To construct scenarios and strategies, we need such simple and rational tools in order to stimulate imagination, to improve coherence and to facilitate appropriation.</t>
+  </si>
+  <si>
+    <t>The future is multiple and several potential futures are possible; the path leading to this or that future is not necessarily unique., The description of a potential future and of the progression towqards it comprises a 'scenario'</t>
+  </si>
+  <si>
+    <t>What is a scenario? "A description of a future situation and the course of events which allows one to move forward from the original situation to the future situation". Two major categories of scenario can be identified: Exploratory: starting from past and present trends and leading to a likely future; Anticipatory or normative: built on the basis of different visions of the future. they may be either desired or, on the contrary, feared.</t>
+  </si>
+  <si>
+    <t>Classically, a distinction is made between the following: possible scenarios, ie, everything that can be imaged; realisable scenarios. Ie, all that is possible, taking account of constraints; desirable scenarios, ie, which fall into the possible category, but which are not all necessarily realisable.</t>
+  </si>
+  <si>
+    <t>In principle, a trend-based scenario, whether or not it is probable, corresponds to the extrapolation of trends at all points where choices are to be made. It is among the realizable scenarios, which have a higher than zero probability, that we find contrasted (unlikely) scenarios and the field of development where the most probable scenarios are found. As regards desirable scenarios, these are found certainwhere within the possible zone, and are not all necessarly realizable.</t>
+  </si>
+  <si>
+    <t>There is often confusion between scenarios and strategies. While scenarios depend on the type of vision adopted (exploratory, normative or retroprojective) and on probability, strategies depend on attitudes adopted in the face of possible futures.</t>
+  </si>
+  <si>
+    <t>Características dos cenários</t>
+  </si>
+  <si>
+    <t>Futuro</t>
+  </si>
+  <si>
+    <t>Caracteristica</t>
+  </si>
+  <si>
+    <t>Forecast porque não usar</t>
+  </si>
+  <si>
+    <t>Como construir</t>
+  </si>
+  <si>
+    <t>We recall that the hypotheses must simultaneously comply with the three prerequisite conditions, viz., relevance, coherence and likelihood.</t>
+  </si>
+  <si>
+    <t>Tipos</t>
+  </si>
+  <si>
+    <t>Diferença entre cenários e estratégia</t>
+  </si>
+  <si>
+    <t>The art of scenarios and strategic planning: tools and pitfalls</t>
+  </si>
+  <si>
+    <t>@article{Godet2010-AoS,
+  author = {Godet, Michel},
+  doi = {10.1016/S0040-1625(99)00120-1},
+  issn = {0040-1625},
+  journal = {Technological Forecasting and Social Change},
+  month = sep,
+  number = 1,
+  pages = {3--22},
+  shorttitle = {The Art of Scenarios and Strategic Planning},
+  timestamp = {2010-06-13T21:13:34.000+0200},
+  title = {{The Art of Scenarios and Strategic Planning: Tools and Pitfalls}},
+  url = {http://www.sciencedirect.com/science/article/B6V71-41C2TXX-2/2/2b78fbf31851b872c3a15b693fd46300},
+  volume = 65,
+  year = 2000
+}</t>
+  </si>
+  <si>
+    <t>Anticipation is not widely practived by decision makers because when things are going well, they can manage without it, and when things are going badly, it is too late to see beyound the ends of their noses.</t>
+  </si>
+  <si>
+    <t>Action becomes meaningless without a goal, and only anticipation points the way to action and gives it both meaning and direction.</t>
+  </si>
+  <si>
+    <t>Necessidade</t>
+  </si>
+  <si>
+    <t>Continuing the tradition of strategic planning and strategic management, strategic prospective emphasizes the importance of long-range and alternative thinking in strategic decision-making process.</t>
+  </si>
+  <si>
+    <t>Planejamento estratégico prospectivo</t>
+  </si>
+  <si>
+    <t>Intuition and reason are not opposite, but complementary faculties. People cannot be reduced to a rational mind (the left hemisphere); they are also driven bu the emotional faculties (the right hemisphere) It is time we stopped opposing intuitive vision and rational thinking, because both are necessary.</t>
+  </si>
+  <si>
+    <t>What has been rediscovered with strategic management is that people and organizations are at the heart of the difference between efficient and inefficient firms.</t>
+  </si>
+  <si>
+    <t>Origem das mudanças</t>
+  </si>
+  <si>
+    <t>The rich heritage of strategic analysis remains with us. For example, the classical analysis using threats and opportunities coming from the general environment shows that we canot limit our analysis to the competitive enrironment int the name of short-term profits, as the early weritings of Michael Porter might lead us to believe [5]. The fact that many uncertainties hang in the balance within the general context, especially over the long term, underscores the need for broad scenario buyilding to clarify the strategic options available and to ensure continued development.</t>
+  </si>
+  <si>
+    <t>Strategy uses foresight and innovation; whereas prospective uses preactivity and proactivity, but we are talking about the exact same thing.</t>
+  </si>
+  <si>
+    <t>By now we are convinced that la prospective is often strategic, if not through its outcome at least through its intentions and, similarly, strategy calls upon prospective to clarify choices made with the future in mind.</t>
+  </si>
+  <si>
+    <t>Motivação</t>
+  </si>
+  <si>
+    <t>In reality, the issue is not really planning, buyt rather the manner in which planning is carried out. The graft of strategic planning only takes root if it is integrated into the corporate culture and identity.</t>
+  </si>
+  <si>
+    <t>The main advantage of these rigid definitions is that they avoid the use of the word strategic to qualify anything that seemd important.</t>
+  </si>
+  <si>
+    <t>Planejamento estratégico prospectivo - falando sobre colocar o nome estrategico em qualquer coisa para parecer que ele é importante.</t>
+  </si>
+  <si>
+    <t>It is, therefore, prudent to separate na exploratory phase of identification of future stakes from a normative phase. A normative phase is required to define strategic choices, in other words, choices that are possible and desirable in order to keep on course. The distinction between these two phases is all the more justified in that the choice of strategies is conditioned by the uncertainty weighing on the scenarios and by the contrast among the most probable of them.</t>
+  </si>
+  <si>
+    <t>Tipos de cenários de futuro</t>
+  </si>
+  <si>
+    <t>The uncertainty of the future can be appraised through the number of possible scenarios within the field of probables., In principle, the higher the number, the greater the uncertainty. This is in principle only, however, because the difference in content vrtween the scenarios must also be considered: the most probable can be very similar or highly contrasted. Experience shows thet, in general, a third of the total possible scenarios is enough to cover 80% of the field of probables; ie., 10 scenarios out of 32 possibles for five fundamental hypotheses. (it may change whe this amount is higher os lower).</t>
+  </si>
+  <si>
+    <t>Número de cenários</t>
+  </si>
+  <si>
+    <t>Like two lovers locked in an embrace, prospective and strategy remain distinct entities, and it is necessary to distinguish between: (1) - a time for anticipation, in other words, the study of possible and desirable changes; and (2) a time to prepare action: in other words, the working out and assessing of possible strategic choices so as to be prepared for expected changes (preactivity) and provoke desirable changes (proactivity). The dichotomy between exploring and preparing a course of action implies the five following questions: (Q1) what can and might happen? (Q2) what can I do? (Q3) what am I going to do? (Q4) how am I going to do it? and an essential prequestion (Q0) who am I? All too often ignored, the last question is the starting point.</t>
+  </si>
+  <si>
+    <t>Diferença entre prospectiva e estratégia</t>
+  </si>
+  <si>
+    <t>For the sake of clarity, the expression "strategic prospective" will, therefore, be reserved for futures studies having strategic ambitions and end points for those undertaking them.</t>
+  </si>
+  <si>
+    <t>Prospectiva e estratégia</t>
+  </si>
+  <si>
+    <t>A scenario is the set formed by the description of a future situation and the course of events that enables on to progress from the original situation to the future situation. The word scenario is often abused, especially when used to describe any set of hypotheses. Of course, these hypotheses must simultaneously be pertinent, coherent, plausible, important, and transparent to meet all our critertia. Two major categories of scenarios can be identified: (1) exploratory: starting from past and present trends and leading to likely futures; and (2) anticipatory or normative: built on the basis of alternative visions of the future they may be desired or, on the contrary, feared. They have been designed "retroprofectively". These exploratory or anticipatory scenarios can, moreover, indiate a trend or be contrasted, depending on whether they take into account the most likely or extreme developments.</t>
+  </si>
+  <si>
+    <t>Prospective remains na art that requires several other talents to succeed, for example, conformism, intuition, and common sense.</t>
+  </si>
+  <si>
+    <t>Talentos</t>
+  </si>
+  <si>
+    <t>If anticipation really is to serve action, it must no longer be an art reserved for enlightened princes but rather a matter for the majority. Everyone of us should be concerned about the future, because that is where we will be spending the rest of our lives. If there is no appropriation, there is only rejection. The best ideas are not the ones that we have, but rather the ones that we initiate in others. Motivating people and managerial talent make the difference between successful firms or regions and those that crumble.</t>
   </si>
 </sst>
 </file>
@@ -1190,7 +1350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1252,14 +1412,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1575,28 +1738,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J141"/>
+  <dimension ref="A1:K170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13:I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="72.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="4.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="4.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="233.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.875" style="5"/>
+    <col min="8" max="8" width="32.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="126.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="233.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1628,7 +1791,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="42" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1650,7 +1813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="70" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1671,7 +1834,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="56" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1695,7 +1858,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="42" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1719,7 +1882,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="84" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1740,7 +1903,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="102" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1758,7 +1921,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="42" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1779,7 +1942,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="56" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1800,7 +1963,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="154" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1821,7 +1984,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="154" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1842,7 +2005,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="140" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -1866,7 +2029,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="28" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
@@ -1886,8 +2049,11 @@
       <c r="H13" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+      <c r="I13" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="98" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -1907,8 +2073,11 @@
       <c r="H14" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="I14" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="28" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -1924,8 +2093,11 @@
       <c r="H15" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="I15" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="56" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>36</v>
       </c>
@@ -1944,8 +2116,11 @@
       <c r="H16" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="I16" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="56" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
@@ -1964,8 +2139,11 @@
       <c r="H17" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="I17" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="126" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
@@ -1984,8 +2162,11 @@
       <c r="H18" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="I18" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="42" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -2004,8 +2185,11 @@
       <c r="H19" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="I19" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="126" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
@@ -2024,8 +2208,11 @@
       <c r="H20" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="I20" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="56" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
@@ -2044,8 +2231,11 @@
       <c r="H21" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="I21" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>36</v>
       </c>
@@ -2061,8 +2251,11 @@
       <c r="H22" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="I22" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>36</v>
       </c>
@@ -2078,8 +2271,11 @@
       <c r="H23" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="102" x14ac:dyDescent="0.25">
+      <c r="I23" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
@@ -2095,8 +2291,11 @@
       <c r="H24" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="102" x14ac:dyDescent="0.25">
+      <c r="I24" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>36</v>
       </c>
@@ -2112,8 +2311,11 @@
       <c r="H25" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="I25" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="42" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>36</v>
       </c>
@@ -2132,8 +2334,11 @@
       <c r="H26" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="I26" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="98" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>36</v>
       </c>
@@ -2152,8 +2357,11 @@
       <c r="H27" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="I27" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="84" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>36</v>
       </c>
@@ -2172,8 +2380,11 @@
       <c r="H28" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="I28" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>36</v>
       </c>
@@ -2192,8 +2403,11 @@
       <c r="H29" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="I29" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="84" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>36</v>
       </c>
@@ -2212,8 +2426,11 @@
       <c r="H30" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="51" x14ac:dyDescent="0.25">
+      <c r="I30" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="98" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
@@ -2232,8 +2449,11 @@
       <c r="H31" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="229.5" x14ac:dyDescent="0.25">
+      <c r="I31" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="252" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
@@ -2243,8 +2463,11 @@
       <c r="G32" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="I32" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="140" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -2263,8 +2486,11 @@
       <c r="H33" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="I33" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="98" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>101</v>
       </c>
@@ -2284,7 +2510,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="98" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>101</v>
       </c>
@@ -2301,7 +2527,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="70" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>101</v>
       </c>
@@ -2318,7 +2544,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" s="9" customFormat="1" ht="70" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>113</v>
       </c>
@@ -2339,7 +2565,7 @@
       </c>
       <c r="J37" s="8"/>
     </row>
-    <row r="38" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" s="9" customFormat="1" ht="28" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>113</v>
       </c>
@@ -2355,10 +2581,12 @@
       <c r="H38" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="I38" s="8"/>
+      <c r="I38" s="8" t="s">
+        <v>210</v>
+      </c>
       <c r="J38" s="8"/>
     </row>
-    <row r="39" spans="1:10" s="9" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" s="9" customFormat="1" ht="168" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>113</v>
       </c>
@@ -2374,10 +2602,12 @@
       <c r="H39" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="I39" s="8"/>
+      <c r="I39" s="8" t="s">
+        <v>210</v>
+      </c>
       <c r="J39" s="8"/>
     </row>
-    <row r="40" spans="1:10" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" s="9" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>113</v>
       </c>
@@ -2391,19 +2621,24 @@
       <c r="H40" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="I40" s="8"/>
+      <c r="I40" s="8" t="s">
+        <v>210</v>
+      </c>
       <c r="J40" s="8"/>
     </row>
-    <row r="41" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
+    <row r="41" spans="1:10" ht="84" x14ac:dyDescent="0.2">
+      <c r="A41" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="23" t="s">
+      <c r="I41" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="70" x14ac:dyDescent="0.2">
+      <c r="A42" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D42" s="2" t="s">
@@ -2415,9 +2650,12 @@
       <c r="H42" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="23" t="s">
+      <c r="I42" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="140" x14ac:dyDescent="0.2">
+      <c r="A43" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D43" s="2" t="s">
@@ -2429,9 +2667,12 @@
       <c r="H43" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="23" t="s">
+      <c r="I43" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="70" x14ac:dyDescent="0.2">
+      <c r="A44" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D44" s="2" t="s">
@@ -2443,9 +2684,12 @@
       <c r="H44" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="23" t="s">
+      <c r="I44" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="140" x14ac:dyDescent="0.2">
+      <c r="A45" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D45" s="2" t="s">
@@ -2457,9 +2701,12 @@
       <c r="H45" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="23" t="s">
+      <c r="I45" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="56" x14ac:dyDescent="0.2">
+      <c r="A46" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -2471,9 +2718,12 @@
       <c r="H46" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="23" t="s">
+      <c r="I46" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="42" x14ac:dyDescent="0.2">
+      <c r="A47" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D47" s="2" t="s">
@@ -2485,9 +2735,12 @@
       <c r="H47" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A48" s="23" t="s">
+      <c r="I47" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="84" x14ac:dyDescent="0.2">
+      <c r="A48" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D48" s="2" t="s">
@@ -2499,9 +2752,12 @@
       <c r="H48" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="23" t="s">
+      <c r="I48" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="84" x14ac:dyDescent="0.2">
+      <c r="A49" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D49" s="2" t="s">
@@ -2513,9 +2769,12 @@
       <c r="H49" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="23" t="s">
+      <c r="I49" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="98" x14ac:dyDescent="0.2">
+      <c r="A50" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -2527,9 +2786,12 @@
       <c r="H50" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="23" t="s">
+      <c r="I50" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="56" x14ac:dyDescent="0.2">
+      <c r="A51" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D51" s="2" t="s">
@@ -2541,9 +2803,12 @@
       <c r="H51" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A52" s="23" t="s">
+      <c r="I51" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="98" x14ac:dyDescent="0.2">
+      <c r="A52" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D52" s="2" t="s">
@@ -2555,9 +2820,12 @@
       <c r="H52" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A53" s="23" t="s">
+      <c r="I52" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="196" x14ac:dyDescent="0.2">
+      <c r="A53" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D53" s="2" t="s">
@@ -2569,9 +2837,12 @@
       <c r="H53" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" ht="242.25" x14ac:dyDescent="0.25">
-      <c r="A54" s="23" t="s">
+      <c r="I53" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A54" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D54" s="2" t="s">
@@ -2583,9 +2854,12 @@
       <c r="H54" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A55" s="23" t="s">
+      <c r="I54" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="70" x14ac:dyDescent="0.2">
+      <c r="A55" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D55" s="2" t="s">
@@ -2597,9 +2871,12 @@
       <c r="H55" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="102" x14ac:dyDescent="0.25">
-      <c r="A56" s="23" t="s">
+      <c r="I55" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="210" x14ac:dyDescent="0.2">
+      <c r="A56" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D56" s="2" t="s">
@@ -2611,9 +2888,12 @@
       <c r="H56" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A57" s="23" t="s">
+      <c r="I56" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="98" x14ac:dyDescent="0.2">
+      <c r="A57" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D57" s="2" t="s">
@@ -2625,9 +2905,12 @@
       <c r="H57" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="23" t="s">
+      <c r="I57" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="70" x14ac:dyDescent="0.2">
+      <c r="A58" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D58" s="2" t="s">
@@ -2639,9 +2922,12 @@
       <c r="H58" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="23" t="s">
+      <c r="I58" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="140" x14ac:dyDescent="0.2">
+      <c r="A59" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D59" s="2" t="s">
@@ -2653,9 +2939,12 @@
       <c r="H59" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="23" t="s">
+      <c r="I59" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="140" x14ac:dyDescent="0.2">
+      <c r="A60" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D60" s="2" t="s">
@@ -2667,9 +2956,12 @@
       <c r="H60" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="23" t="s">
+      <c r="I60" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="42" x14ac:dyDescent="0.2">
+      <c r="A61" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D61" s="2" t="s">
@@ -2681,9 +2973,12 @@
       <c r="H61" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="204" x14ac:dyDescent="0.25">
-      <c r="A62" s="23" t="s">
+      <c r="I61" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="345" x14ac:dyDescent="0.2">
+      <c r="A62" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D62" s="2" t="s">
@@ -2695,9 +2990,12 @@
       <c r="H62" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="23" t="s">
+      <c r="I62" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="56" x14ac:dyDescent="0.2">
+      <c r="A63" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D63" s="2" t="s">
@@ -2709,9 +3007,12 @@
       <c r="H63" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="23" t="s">
+      <c r="I63" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="56" x14ac:dyDescent="0.2">
+      <c r="A64" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D64" s="2" t="s">
@@ -2723,9 +3024,12 @@
       <c r="H64" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" ht="153" x14ac:dyDescent="0.25">
-      <c r="A65" s="23" t="s">
+      <c r="I64" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="266" x14ac:dyDescent="0.2">
+      <c r="A65" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D65" s="2" t="s">
@@ -2737,9 +3041,12 @@
       <c r="H65" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A66" s="23" t="s">
+      <c r="I65" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+      <c r="A66" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D66" s="2" t="s">
@@ -2751,9 +3058,12 @@
       <c r="H66" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A67" s="23" t="s">
+      <c r="I66" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+      <c r="A67" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D67" s="2" t="s">
@@ -2765,9 +3075,12 @@
       <c r="H67" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="23" t="s">
+      <c r="I67" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A68" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D68" s="2" t="s">
@@ -2779,9 +3092,12 @@
       <c r="H68" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A69" s="23" t="s">
+      <c r="I68" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="182" x14ac:dyDescent="0.2">
+      <c r="A69" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D69" s="2" t="s">
@@ -2793,9 +3109,12 @@
       <c r="H69" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="23" t="s">
+      <c r="I69" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="56" x14ac:dyDescent="0.2">
+      <c r="A70" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D70" s="2" t="s">
@@ -2807,9 +3126,12 @@
       <c r="H70" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="23" t="s">
+      <c r="I70" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="252" x14ac:dyDescent="0.2">
+      <c r="A71" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D71" s="2" t="s">
@@ -2821,9 +3143,12 @@
       <c r="H71" s="2" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A72" s="23" t="s">
+      <c r="I71" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="98" x14ac:dyDescent="0.2">
+      <c r="A72" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D72" s="2" t="s">
@@ -2835,9 +3160,12 @@
       <c r="H72" s="2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="23" t="s">
+      <c r="I72" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="70" x14ac:dyDescent="0.2">
+      <c r="A73" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D73" s="2" t="s">
@@ -2849,9 +3177,12 @@
       <c r="H73" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" ht="102" x14ac:dyDescent="0.25">
-      <c r="A74" s="23" t="s">
+      <c r="I73" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="210" x14ac:dyDescent="0.2">
+      <c r="A74" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D74" s="2" t="s">
@@ -2863,9 +3194,12 @@
       <c r="H74" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="23" t="s">
+      <c r="I74" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="42" x14ac:dyDescent="0.2">
+      <c r="A75" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D75" s="2" t="s">
@@ -2877,9 +3211,12 @@
       <c r="H75" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="23" t="s">
+      <c r="I75" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="168" x14ac:dyDescent="0.2">
+      <c r="A76" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D76" s="2" t="s">
@@ -2891,9 +3228,12 @@
       <c r="H76" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A77" s="23" t="s">
+      <c r="I76" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="84" x14ac:dyDescent="0.2">
+      <c r="A77" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D77" s="2" t="s">
@@ -2905,9 +3245,12 @@
       <c r="H77" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A78" s="23" t="s">
+      <c r="I77" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="84" x14ac:dyDescent="0.2">
+      <c r="A78" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D78" s="2" t="s">
@@ -2919,9 +3262,12 @@
       <c r="H78" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A79" s="23" t="s">
+      <c r="I78" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="84" x14ac:dyDescent="0.2">
+      <c r="A79" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D79" s="2" t="s">
@@ -2933,9 +3279,12 @@
       <c r="H79" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" ht="51" x14ac:dyDescent="0.25">
-      <c r="A80" s="23" t="s">
+      <c r="I79" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+      <c r="A80" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D80" s="2" t="s">
@@ -2947,9 +3296,12 @@
       <c r="H80" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="23" t="s">
+      <c r="I80" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="126" x14ac:dyDescent="0.2">
+      <c r="A81" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D81" s="11" t="s">
@@ -2961,9 +3313,12 @@
       <c r="H81" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="23" t="s">
+      <c r="I81" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="84" x14ac:dyDescent="0.2">
+      <c r="A82" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D82" s="2" t="s">
@@ -2975,9 +3330,12 @@
       <c r="H82" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" ht="51" x14ac:dyDescent="0.25">
-      <c r="A83" s="23" t="s">
+      <c r="I82" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+      <c r="A83" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D83" s="2" t="s">
@@ -2989,9 +3347,12 @@
       <c r="H83" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" ht="178.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="23" t="s">
+      <c r="I83" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="358" x14ac:dyDescent="0.2">
+      <c r="A84" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D84" s="2" t="s">
@@ -3003,9 +3364,12 @@
       <c r="H84" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A85" s="23" t="s">
+      <c r="I84" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="84" x14ac:dyDescent="0.2">
+      <c r="A85" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D85" s="2" t="s">
@@ -3017,8 +3381,11 @@
       <c r="H85" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="I85" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="70" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>185</v>
       </c>
@@ -3035,7 +3402,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="168" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>185</v>
       </c>
@@ -3052,7 +3419,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="182" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>185</v>
       </c>
@@ -3069,7 +3436,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="98" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>185</v>
       </c>
@@ -3086,7 +3453,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>185</v>
       </c>
@@ -3103,7 +3470,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="98" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>185</v>
       </c>
@@ -3120,7 +3487,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="70" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>185</v>
       </c>
@@ -3137,7 +3504,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="98" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>185</v>
       </c>
@@ -3154,7 +3521,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="154" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>185</v>
       </c>
@@ -3171,7 +3538,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="168" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>185</v>
       </c>
@@ -3188,7 +3555,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="140" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>185</v>
       </c>
@@ -3205,7 +3572,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="56" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>185</v>
       </c>
@@ -3222,7 +3589,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="182" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>185</v>
       </c>
@@ -3239,7 +3606,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="98" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>185</v>
       </c>
@@ -3256,7 +3623,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="126" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>185</v>
       </c>
@@ -3273,7 +3640,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="182" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>212</v>
       </c>
@@ -3290,7 +3657,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>212</v>
       </c>
@@ -3307,7 +3674,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="84" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>212</v>
       </c>
@@ -3324,7 +3691,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="98" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>212</v>
       </c>
@@ -3341,7 +3708,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="84" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>212</v>
       </c>
@@ -3358,7 +3725,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="70" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>212</v>
       </c>
@@ -3375,7 +3742,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="98" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>212</v>
       </c>
@@ -3392,7 +3759,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="56" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>212</v>
       </c>
@@ -3409,7 +3776,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>212</v>
       </c>
@@ -3426,7 +3793,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>212</v>
       </c>
@@ -3443,7 +3810,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" ht="266" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>212</v>
       </c>
@@ -3460,7 +3827,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="140" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>212</v>
       </c>
@@ -3477,7 +3844,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="140" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>212</v>
       </c>
@@ -3494,7 +3861,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" ht="98" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>212</v>
       </c>
@@ -3511,7 +3878,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" ht="70" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>212</v>
       </c>
@@ -3528,7 +3895,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" ht="210" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>212</v>
       </c>
@@ -3545,7 +3912,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>212</v>
       </c>
@@ -3562,7 +3929,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>212</v>
       </c>
@@ -3579,7 +3946,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" ht="98" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>212</v>
       </c>
@@ -3596,7 +3963,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" ht="154" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>212</v>
       </c>
@@ -3613,7 +3980,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>212</v>
       </c>
@@ -3630,7 +3997,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" ht="168" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>212</v>
       </c>
@@ -3647,7 +4014,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" ht="140" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>212</v>
       </c>
@@ -3664,7 +4031,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>212</v>
       </c>
@@ -3681,7 +4048,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" ht="154" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>212</v>
       </c>
@@ -3698,7 +4065,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" ht="112" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>212</v>
       </c>
@@ -3715,7 +4082,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" ht="140" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>212</v>
       </c>
@@ -3732,7 +4099,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" ht="98" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>212</v>
       </c>
@@ -3749,7 +4116,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" ht="140" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>212</v>
       </c>
@@ -3766,7 +4133,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" ht="182" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>212</v>
       </c>
@@ -3783,7 +4150,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" ht="140" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>212</v>
       </c>
@@ -3800,7 +4167,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" ht="126" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>212</v>
       </c>
@@ -3817,7 +4184,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" ht="154" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>212</v>
       </c>
@@ -3834,7 +4201,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="102" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" ht="84" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>284</v>
       </c>
@@ -3851,7 +4218,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="382.5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>284</v>
       </c>
@@ -3868,7 +4235,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" ht="42" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>284</v>
       </c>
@@ -3885,7 +4252,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" ht="42" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>284</v>
       </c>
@@ -3902,7 +4269,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="165.75" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" ht="182" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>284</v>
       </c>
@@ -3919,7 +4286,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>284</v>
       </c>
@@ -3936,7 +4303,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" ht="126" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>284</v>
       </c>
@@ -3953,12 +4320,498 @@
         <v>285</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>298</v>
       </c>
+      <c r="B141" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="G141" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H141" s="2" t="s">
+        <v>312</v>
+      </c>
       <c r="I141" s="4" t="s">
         <v>299</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="28" x14ac:dyDescent="0.2">
+      <c r="A142" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="G142" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H142" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="I142" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="98" x14ac:dyDescent="0.2">
+      <c r="A143" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G143" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H143" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="I143" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" ht="70" x14ac:dyDescent="0.2">
+      <c r="A144" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="G144" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H144" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="I144" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" ht="70" x14ac:dyDescent="0.2">
+      <c r="A145" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="G145" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H145" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="I145" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" ht="56" x14ac:dyDescent="0.2">
+      <c r="A146" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="I146" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" ht="28" x14ac:dyDescent="0.2">
+      <c r="A147" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G147" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H147" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="I147" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" ht="42" x14ac:dyDescent="0.2">
+      <c r="A148" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G148" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H148" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I148" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" ht="70" x14ac:dyDescent="0.2">
+      <c r="A149" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="G149" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H149" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="I149" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" ht="28" x14ac:dyDescent="0.2">
+      <c r="A150" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="I150" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" ht="56" x14ac:dyDescent="0.2">
+      <c r="A151" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="G151" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H151" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="I151" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" ht="84" x14ac:dyDescent="0.2">
+      <c r="A152" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="G152" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H152" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="I152" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" ht="42" x14ac:dyDescent="0.2">
+      <c r="A153" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="G153" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H153" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="I153" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" ht="42" x14ac:dyDescent="0.2">
+      <c r="A154" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="G154" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H154" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I154" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="J154" s="5"/>
+      <c r="K154" s="4"/>
+    </row>
+    <row r="155" spans="1:11" ht="28" x14ac:dyDescent="0.2">
+      <c r="A155" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="G155" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H155" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="I155" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" ht="42" x14ac:dyDescent="0.2">
+      <c r="A156" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="G156" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H156" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="I156" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" ht="56" x14ac:dyDescent="0.2">
+      <c r="A157" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="G157" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H157" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="I157" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" ht="28" x14ac:dyDescent="0.2">
+      <c r="A158" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="G158" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H158" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="I158" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" ht="98" x14ac:dyDescent="0.2">
+      <c r="A159" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="G159" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H159" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="I159" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" ht="28" x14ac:dyDescent="0.2">
+      <c r="A160" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="G160" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H160" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I160" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" ht="42" x14ac:dyDescent="0.2">
+      <c r="A161" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="G161" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H161" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="I161" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" ht="42" x14ac:dyDescent="0.2">
+      <c r="A162" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="G162" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H162" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="I162" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" ht="56" x14ac:dyDescent="0.2">
+      <c r="A163" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="G163" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H163" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="I163" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" ht="84" x14ac:dyDescent="0.2">
+      <c r="A164" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="G164" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H164" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="I164" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" ht="98" x14ac:dyDescent="0.2">
+      <c r="A165" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="G165" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H165" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="I165" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" ht="126" x14ac:dyDescent="0.2">
+      <c r="A166" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="G166" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H166" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="I166" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" ht="28" x14ac:dyDescent="0.2">
+      <c r="A167" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="G167" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H167" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="I167" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" ht="154" x14ac:dyDescent="0.2">
+      <c r="A168" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="G168" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H168" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="I168" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" ht="28" x14ac:dyDescent="0.2">
+      <c r="A169" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="G169" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H169" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="I169" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" ht="98" x14ac:dyDescent="0.2">
+      <c r="A170" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="I170" s="4" t="s">
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -3976,28 +4829,28 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="27.375" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="21.25" style="12" customWidth="1"/>
-    <col min="5" max="5" width="25.625" style="12" customWidth="1"/>
-    <col min="6" max="7" width="21.25" style="12" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21.1640625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" style="12" customWidth="1"/>
+    <col min="6" max="7" width="21.1640625" style="12" customWidth="1"/>
     <col min="8" max="16384" width="13.5" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.25">
       <c r="A1" s="19"/>
       <c r="B1" s="19"/>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-    </row>
-    <row r="2" spans="1:7" s="14" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+    </row>
+    <row r="2" spans="1:7" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="19"/>
       <c r="B2" s="20"/>
       <c r="C2" s="17" t="s">
@@ -4016,8 +4869,8 @@
         <v>253</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
         <v>254</v>
       </c>
       <c r="B3" s="18" t="s">
@@ -4039,8 +4892,8 @@
         <v>260</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
+    <row r="4" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="23"/>
       <c r="B4" s="18" t="s">
         <v>256</v>
       </c>
@@ -4060,8 +4913,8 @@
         <v>260</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
+    <row r="5" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="23"/>
       <c r="B5" s="18" t="s">
         <v>257</v>
       </c>
@@ -4081,8 +4934,8 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
+    <row r="6" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="23"/>
       <c r="B6" s="18" t="s">
         <v>258</v>
       </c>
@@ -4102,8 +4955,8 @@
         <v>260</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
+    <row r="7" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="23"/>
       <c r="B7" s="18" t="s">
         <v>259</v>
       </c>

</xml_diff>

<commit_message>
Terminado mais um artigo e atualização do fichamento
</commit_message>
<xml_diff>
--- a/FICHAMENTO.xlsx
+++ b/FICHAMENTO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigosantos/Documents/GitHub/weak_signals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053CAD05-14E6-954B-B737-CEFC871C6519}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B9EC16-B36B-F049-99C1-91A4A47273FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5000" yWindow="-21140" windowWidth="38260" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="365">
   <si>
     <t>Título</t>
   </si>
@@ -1256,6 +1256,63 @@
   </si>
   <si>
     <t>If anticipation really is to serve action, it must no longer be an art reserved for enlightened princes but rather a matter for the majority. Everyone of us should be concerned about the future, because that is where we will be spending the rest of our lives. If there is no appropriation, there is only rejection. The best ideas are not the ones that we have, but rather the ones that we initiate in others. Motivating people and managerial talent make the difference between successful firms or regions and those that crumble.</t>
+  </si>
+  <si>
+    <t>@article{article,
+author = {Durance, Philippe and Godet, Michel},
+year = {2010},
+month = {11},
+pages = {1488-1492},
+title = {Scenario building: Uses and abuses},
+volume = {77},
+journal = {Technological Forecasting and Social Change - TECHNOL FORECAST SOC CHANGE},
+doi = {10.1016/j.techfore.2010.06.007}
+}</t>
+  </si>
+  <si>
+    <t>Scenario building: Uses and abuses</t>
+  </si>
+  <si>
+    <t>A scenario is not a future reality but rather a means to represent it with the aim of clarifying present action in light of possible and desirable futures.</t>
+  </si>
+  <si>
+    <t>Thus, without a careful and attentive reader, many scenarios pass as credible as if the reader is guilty of not having understood the underlying meaning.</t>
+  </si>
+  <si>
+    <t>A scenario is a description (usually of a possble future) which assumes the intervention of several key events or conditions which will have taken place between the time of the original situation and the time in which the scwenario is set.</t>
+  </si>
+  <si>
+    <t>A scenario must satisfy the following conditions: pertinence, coherence, likelihood, importance and transparency.</t>
+  </si>
+  <si>
+    <t>Exploratory scenarios are concerned with past and present trends and lead to likely futures., Normative scenarios are constructed from alternative images of the future which may be both desirable and feare, and are conceived in a retro projective way. Thus, exploratory scenarios are devoid of human values, ewhereas normative scenarios are the expression of human values.</t>
+  </si>
+  <si>
+    <t>A scenario is not and end in itself. I only has meaning as na aid to decision-making in so far as it clarifies the consequences of current decisions.</t>
+  </si>
+  <si>
+    <t>Scenario splanning requires time to be done right, and a 12- to 18-month timeframe is not rare. Time is needed in prospective and strategic diagnoses so that scenarios involving the environment may be developed and that the main stakes for a specific organization based on possible futures, as revealed by scenarios, may be reviewed.</t>
+  </si>
+  <si>
+    <t>As a result, it is important to gather as many informed judgments as possible and then forge a consensus.</t>
+  </si>
+  <si>
+    <t>The uncertainty of the future can be evaluated across a number of scenarios which share he field of probable futures.</t>
+  </si>
+  <si>
+    <t>However, it is imporatnt to take into consideration the content of the various scenarios since the more probable among them may be either very similar or quite contrasted to one another. In theory, two possible situations may present themselves.</t>
+  </si>
+  <si>
+    <t>Using morphological analysis, a global system can be decomposed into dimensions (key questions concerning the future). Theses dimensions are: demographis, economic, technological, and social/organizational.</t>
+  </si>
+  <si>
+    <t>Prazo</t>
+  </si>
+  <si>
+    <t>In extreme cases, policy-makers may launch a Foresight study that they wish to see finished in a matter of weeks. In this event, the prevailing conditions are rarely ideal, thought it is better to light a candle than curse the darkness.</t>
+  </si>
+  <si>
+    <t>Given a short time-frame, it is often advisable to limit the scenarios to several key hypotheses, say four to six.</t>
   </si>
 </sst>
 </file>
@@ -1415,14 +1472,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1738,10 +1795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K170"/>
+  <dimension ref="A1:K183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13:I33"/>
+    <sheetView tabSelected="1" topLeftCell="C168" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I187" sqref="I187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1882,7 +1939,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="84" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="98" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -2527,7 +2584,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="70" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="84" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>101</v>
       </c>
@@ -2633,7 +2690,7 @@
       <c r="D41" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I41" s="24" t="s">
+      <c r="I41" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2650,7 +2707,7 @@
       <c r="H42" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="I42" s="24" t="s">
+      <c r="I42" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2667,7 +2724,7 @@
       <c r="H43" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="I43" s="24" t="s">
+      <c r="I43" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2684,7 +2741,7 @@
       <c r="H44" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I44" s="24" t="s">
+      <c r="I44" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2701,7 +2758,7 @@
       <c r="H45" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="I45" s="24" t="s">
+      <c r="I45" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2718,7 +2775,7 @@
       <c r="H46" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="I46" s="24" t="s">
+      <c r="I46" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2735,7 +2792,7 @@
       <c r="H47" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="I47" s="24" t="s">
+      <c r="I47" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2752,7 +2809,7 @@
       <c r="H48" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="I48" s="24" t="s">
+      <c r="I48" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2769,7 +2826,7 @@
       <c r="H49" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="I49" s="24" t="s">
+      <c r="I49" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2786,7 +2843,7 @@
       <c r="H50" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="I50" s="24" t="s">
+      <c r="I50" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2803,7 +2860,7 @@
       <c r="H51" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="I51" s="24" t="s">
+      <c r="I51" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2820,7 +2877,7 @@
       <c r="H52" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="I52" s="24" t="s">
+      <c r="I52" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2837,7 +2894,7 @@
       <c r="H53" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I53" s="24" t="s">
+      <c r="I53" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2854,7 +2911,7 @@
       <c r="H54" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="I54" s="24" t="s">
+      <c r="I54" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2871,7 +2928,7 @@
       <c r="H55" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I55" s="24" t="s">
+      <c r="I55" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2888,7 +2945,7 @@
       <c r="H56" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="I56" s="24" t="s">
+      <c r="I56" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2905,7 +2962,7 @@
       <c r="H57" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="I57" s="24" t="s">
+      <c r="I57" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2922,7 +2979,7 @@
       <c r="H58" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="I58" s="24" t="s">
+      <c r="I58" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2939,7 +2996,7 @@
       <c r="H59" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I59" s="24" t="s">
+      <c r="I59" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2956,7 +3013,7 @@
       <c r="H60" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I60" s="24" t="s">
+      <c r="I60" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2973,7 +3030,7 @@
       <c r="H61" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="I61" s="24" t="s">
+      <c r="I61" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2990,7 +3047,7 @@
       <c r="H62" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="I62" s="24" t="s">
+      <c r="I62" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3007,7 +3064,7 @@
       <c r="H63" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="I63" s="24" t="s">
+      <c r="I63" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3024,7 +3081,7 @@
       <c r="H64" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="I64" s="24" t="s">
+      <c r="I64" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3041,7 +3098,7 @@
       <c r="H65" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="I65" s="24" t="s">
+      <c r="I65" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3058,7 +3115,7 @@
       <c r="H66" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I66" s="24" t="s">
+      <c r="I66" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3075,7 +3132,7 @@
       <c r="H67" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I67" s="24" t="s">
+      <c r="I67" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3092,7 +3149,7 @@
       <c r="H68" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="I68" s="24" t="s">
+      <c r="I68" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3109,7 +3166,7 @@
       <c r="H69" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I69" s="24" t="s">
+      <c r="I69" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3126,7 +3183,7 @@
       <c r="H70" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I70" s="24" t="s">
+      <c r="I70" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3143,7 +3200,7 @@
       <c r="H71" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="I71" s="24" t="s">
+      <c r="I71" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3160,7 +3217,7 @@
       <c r="H72" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="I72" s="24" t="s">
+      <c r="I72" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3177,7 +3234,7 @@
       <c r="H73" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="I73" s="24" t="s">
+      <c r="I73" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3194,7 +3251,7 @@
       <c r="H74" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="I74" s="24" t="s">
+      <c r="I74" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3211,7 +3268,7 @@
       <c r="H75" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="I75" s="24" t="s">
+      <c r="I75" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3228,7 +3285,7 @@
       <c r="H76" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="I76" s="24" t="s">
+      <c r="I76" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3245,7 +3302,7 @@
       <c r="H77" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="I77" s="24" t="s">
+      <c r="I77" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3262,7 +3319,7 @@
       <c r="H78" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="I78" s="24" t="s">
+      <c r="I78" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3279,7 +3336,7 @@
       <c r="H79" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="I79" s="24" t="s">
+      <c r="I79" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3296,7 +3353,7 @@
       <c r="H80" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="I80" s="24" t="s">
+      <c r="I80" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3313,7 +3370,7 @@
       <c r="H81" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="I81" s="24" t="s">
+      <c r="I81" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3330,7 +3387,7 @@
       <c r="H82" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="I82" s="24" t="s">
+      <c r="I82" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3347,7 +3404,7 @@
       <c r="H83" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="I83" s="24" t="s">
+      <c r="I83" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3364,7 +3421,7 @@
       <c r="H84" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="I84" s="24" t="s">
+      <c r="I84" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3381,7 +3438,7 @@
       <c r="H85" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="I85" s="24" t="s">
+      <c r="I85" s="22" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3521,7 +3578,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="154" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="168" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>185</v>
       </c>
@@ -4082,7 +4139,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="140" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" ht="154" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>212</v>
       </c>
@@ -4286,7 +4343,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="28" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9" ht="42" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>284</v>
       </c>
@@ -4803,7 +4860,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="170" spans="1:9" ht="98" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:9" ht="84" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>320</v>
       </c>
@@ -4812,6 +4869,227 @@
       </c>
       <c r="I170" s="4" t="s">
         <v>321</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" ht="28" x14ac:dyDescent="0.2">
+      <c r="A171" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="G171" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H171" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I171" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" ht="28" x14ac:dyDescent="0.2">
+      <c r="A172" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="G172" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H172" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="I172" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" ht="42" x14ac:dyDescent="0.2">
+      <c r="A173" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="G173" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="H173" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I173" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" ht="28" x14ac:dyDescent="0.2">
+      <c r="A174" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="G174" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H174" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="I174" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" ht="70" x14ac:dyDescent="0.2">
+      <c r="A175" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="G175" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H175" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="I175" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" ht="28" x14ac:dyDescent="0.2">
+      <c r="A176" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="G176" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H176" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="I176" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" ht="56" x14ac:dyDescent="0.2">
+      <c r="A177" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G177" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H177" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="I177" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" ht="42" x14ac:dyDescent="0.2">
+      <c r="A178" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="G178" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H178" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="I178" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" ht="28" x14ac:dyDescent="0.2">
+      <c r="A179" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="G179" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H179" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I179" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" ht="28" x14ac:dyDescent="0.2">
+      <c r="A180" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="G180" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H180" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I180" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" ht="28" x14ac:dyDescent="0.2">
+      <c r="A181" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="G181" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H181" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I181" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" ht="42" x14ac:dyDescent="0.2">
+      <c r="A182" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="G182" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H182" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I182" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" ht="42" x14ac:dyDescent="0.2">
+      <c r="A183" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="G183" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H183" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="I183" s="4" t="s">
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -4842,13 +5120,13 @@
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.25">
       <c r="A1" s="19"/>
       <c r="B1" s="19"/>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:7" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="19"/>
@@ -4870,7 +5148,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="24" t="s">
         <v>254</v>
       </c>
       <c r="B3" s="18" t="s">
@@ -4893,7 +5171,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="18" t="s">
         <v>256</v>
       </c>
@@ -4914,7 +5192,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="18" t="s">
         <v>257</v>
       </c>
@@ -4935,7 +5213,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="18" t="s">
         <v>258</v>
       </c>
@@ -4956,7 +5234,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="18" t="s">
         <v>259</v>
       </c>

</xml_diff>

<commit_message>
Atualização nos documentos. Inclusão de novos artigos. Atualização da versão da dissertação.
</commit_message>
<xml_diff>
--- a/FICHAMENTO.xlsx
+++ b/FICHAMENTO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigosantos/Documents/GitHub/weak_signals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C8ECF1-08ED-9046-8BFB-9644FDF28A48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866CA3CD-AEBB-6E49-A426-D25BFA4ACA1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1807,8 +1807,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B76" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView tabSelected="1" topLeftCell="B56" zoomScale="91" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2302,7 +2302,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="409.6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>36</v>
       </c>
@@ -2584,7 +2584,7 @@
       <c r="C35" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="7" t="s">
         <v>108</v>
       </c>
       <c r="G35" s="6" t="s">
@@ -3146,7 +3146,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="21" t="s">
         <v>113</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="252" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" ht="238" x14ac:dyDescent="0.2">
       <c r="A71" s="21" t="s">
         <v>113</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="126" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="126" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="21" t="s">
         <v>113</v>
       </c>
@@ -3388,7 +3388,7 @@
       <c r="A82" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D82" s="7" t="s">
         <v>175</v>
       </c>
       <c r="G82" s="6" t="s">
@@ -3486,7 +3486,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="182" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" ht="168" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>181</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="168" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="154" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>181</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="168" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="154" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>181</v>
       </c>
@@ -3711,7 +3711,7 @@
       <c r="A101" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D101" s="2" t="s">
+      <c r="D101" s="7" t="s">
         <v>209</v>
       </c>
       <c r="G101" s="6" t="s">
@@ -3762,7 +3762,7 @@
       <c r="A104" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D104" s="2" t="s">
+      <c r="D104" s="7" t="s">
         <v>215</v>
       </c>
       <c r="G104" s="6" t="s">
@@ -3779,7 +3779,7 @@
       <c r="A105" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D105" s="2" t="s">
+      <c r="D105" s="7" t="s">
         <v>217</v>
       </c>
       <c r="G105" s="6" t="s">
@@ -3796,7 +3796,7 @@
       <c r="A106" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D106" s="2" t="s">
+      <c r="D106" s="7" t="s">
         <v>219</v>
       </c>
       <c r="G106" s="6" t="s">
@@ -3830,7 +3830,7 @@
       <c r="A108" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D108" s="2" t="s">
+      <c r="D108" s="7" t="s">
         <v>222</v>
       </c>
       <c r="G108" s="6" t="s">
@@ -3847,7 +3847,7 @@
       <c r="A109" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D109" s="2" t="s">
+      <c r="D109" s="7" t="s">
         <v>224</v>
       </c>
       <c r="G109" s="6" t="s">
@@ -3915,7 +3915,7 @@
       <c r="A113" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D113" s="2" t="s">
+      <c r="D113" s="7" t="s">
         <v>230</v>
       </c>
       <c r="G113" s="6" t="s">
@@ -3966,7 +3966,7 @@
       <c r="A116" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D116" s="2" t="s">
+      <c r="D116" s="7" t="s">
         <v>235</v>
       </c>
       <c r="G116" s="6" t="s">
@@ -4102,7 +4102,7 @@
       <c r="A124" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D124" s="2" t="s">
+      <c r="D124" s="7" t="s">
         <v>261</v>
       </c>
       <c r="G124" s="6" t="s">
@@ -4132,7 +4132,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" ht="98" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>208</v>
       </c>
@@ -4149,7 +4149,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="154" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" ht="140" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>208</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="149" spans="1:11" ht="70" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11" ht="70" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>294</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="151" spans="1:11" ht="56" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" ht="56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>294</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="84" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11" ht="84" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>294</v>
       </c>
@@ -4836,7 +4836,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="168" spans="1:9" ht="154" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:9" ht="154" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>316</v>
       </c>
@@ -4949,7 +4949,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="175" spans="1:9" ht="70" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:9" ht="70" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>346</v>
       </c>
@@ -5085,7 +5085,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="183" spans="1:9" ht="42" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:9" ht="42" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
         <v>346</v>
       </c>
@@ -5106,7 +5106,6 @@
   <autoFilter ref="A1:J183" xr:uid="{7C177F3E-3F7D-4913-AABA-E34D03F168B6}">
     <filterColumn colId="7">
       <filters>
-        <filter val="Cenarios - Sinais fracos"/>
         <filter val="S inais Fracos - Processo - Ganhos"/>
         <filter val="Sinais fracos"/>
         <filter val="Sinais Fracos - Aprendizagem Organizacional"/>
@@ -5119,8 +5118,6 @@
         <filter val="Sinais Fracos - Motivações"/>
         <filter val="Sinais Fracos - Processo"/>
         <filter val="Sinais fracos Wild Cards"/>
-        <filter val="Tipos"/>
-        <filter val="Tipos de sinais fracos"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>